<commit_message>
Add "XL Media" figures
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E468"/>
+  <dimension ref="A1:E321"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5590,11 +5590,11 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Бездомный бог. Том 15.</t>
+          <t>Nendoroid Nikki</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>355</v>
+        <v>4553</v>
       </c>
       <c r="D225" t="inlineStr">
         <is>
@@ -5603,7 +5603,7 @@
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Figure</t>
         </is>
       </c>
     </row>
@@ -5613,11 +5613,11 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Росомаха. Полное собрание. Том 1 (Д. Уэй)</t>
+          <t>Nendoroid Amaterasu DX Ver.</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>1315</v>
+        <v>8967</v>
       </c>
       <c r="D226" t="inlineStr">
         <is>
@@ -5626,7 +5626,7 @@
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Figure</t>
         </is>
       </c>
     </row>
@@ -5636,11 +5636,11 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Скитания Эманон. Том 1.</t>
+          <t>Nendoroid Hunter: Male Zinogre Alpha Armor Ver. DX</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>390</v>
+        <v>6295</v>
       </c>
       <c r="D227" t="inlineStr">
         <is>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Figure</t>
         </is>
       </c>
     </row>
@@ -5659,11 +5659,11 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Гостья М. Том 1.</t>
+          <t>Nendoroid Shizue (Isabelle): Winter Ver.</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>580</v>
+        <v>5722</v>
       </c>
       <c r="D228" t="inlineStr">
         <is>
@@ -5672,7 +5672,7 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Figure</t>
         </is>
       </c>
     </row>
@@ -5682,11 +5682,11 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Война миров. Том 1.</t>
+          <t>Nendoroid Orphen</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>370</v>
+        <v>4175</v>
       </c>
       <c r="D229" t="inlineStr">
         <is>
@@ -5695,7 +5695,7 @@
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Figure</t>
         </is>
       </c>
     </row>
@@ -5705,11 +5705,11 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>«Страна чудес смертников». Том 13.</t>
+          <t>Nendoroid Tenya Iida</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>355</v>
+        <v>4594</v>
       </c>
       <c r="D230" t="inlineStr">
         <is>
@@ -5718,7 +5718,7 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Figure</t>
         </is>
       </c>
     </row>
@@ -5728,11 +5728,11 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Евангелион АНИМА. Том 1</t>
+          <t>Nendoroid Ena Saito</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>810</v>
+        <v>7495</v>
       </c>
       <c r="D231" t="inlineStr">
         <is>
@@ -5741,7 +5741,7 @@
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Figure</t>
         </is>
       </c>
     </row>
@@ -5751,11 +5751,11 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Нелюдь. Том 11.</t>
+          <t>Nendoroid Rin Shima: Touring Ver.</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>355</v>
+        <v>6565</v>
       </c>
       <c r="D232" t="inlineStr">
         <is>
@@ -5764,7 +5764,7 @@
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Figure</t>
         </is>
       </c>
     </row>
@@ -5774,11 +5774,11 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>«Страна чудес смертников». Том 12.</t>
+          <t>Nendoroid Sakura Amamiya</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>355</v>
+        <v>4043</v>
       </c>
       <c r="D233" t="inlineStr">
         <is>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Figure</t>
         </is>
       </c>
     </row>
@@ -5797,11 +5797,11 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>«Страна чудес смертников». Том 11.</t>
+          <t>Nendoroid Avenger/Jeanne d'Arc (Alter) Shinjuku Ver.</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>355</v>
+        <v>5892</v>
       </c>
       <c r="D234" t="inlineStr">
         <is>
@@ -5810,7 +5810,7 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Figure</t>
         </is>
       </c>
     </row>
@@ -5820,11 +5820,11 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>«Страна чудес смертников». Том 10.</t>
+          <t>Nendoroid Archer/Gilgamesh: Third Ascension Ver.</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>355</v>
+        <v>5679</v>
       </c>
       <c r="D235" t="inlineStr">
         <is>
@@ -5833,7 +5833,7 @@
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Figure</t>
         </is>
       </c>
     </row>
@@ -5843,11 +5843,11 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Re:Zero. Жизнь с нуля в альтернативном мире. Неделя в особняке. Том 1.</t>
+          <t>Nendoroid Hatsune Miku V4X</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>450</v>
+        <v>6426</v>
       </c>
       <c r="D236" t="inlineStr">
         <is>
@@ -5856,7 +5856,7 @@
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Figure</t>
         </is>
       </c>
     </row>
@@ -5866,11 +5866,11 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Бездомный бог. Том 13.</t>
+          <t>Nendoroid Shinichi Kudo</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>355</v>
+        <v>4161</v>
       </c>
       <c r="D237" t="inlineStr">
         <is>
@@ -5879,7 +5879,7 @@
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Figure</t>
         </is>
       </c>
     </row>
@@ -5889,11 +5889,11 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Бесстрашные защитницы. Том 1. Девы погибели</t>
+          <t>Nendoroid Doll Hatsune Miku</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>445</v>
+        <v>7955</v>
       </c>
       <c r="D238" t="inlineStr">
         <is>
@@ -5902,7 +5902,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Figure</t>
         </is>
       </c>
     </row>
@@ -5912,11 +5912,11 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Гидеон Фолз. Том 1. Чёрный амбар</t>
+          <t>Проза бродячих псов. Том 1.</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>465</v>
+        <v>550</v>
       </c>
       <c r="D239" t="inlineStr">
         <is>
@@ -5935,11 +5935,11 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Тетрадь дружбы Нацумэ. Том 1.</t>
+          <t>Акира. Том 1.</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>550</v>
+        <v>975</v>
       </c>
       <c r="D240" t="inlineStr">
         <is>
@@ -5958,11 +5958,11 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Судьба/Истоки. Том 1.</t>
+          <t>Семь смертных грехов. Том 1.</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>410</v>
+        <v>550</v>
       </c>
       <c r="D241" t="inlineStr">
         <is>
@@ -5981,11 +5981,11 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Рыцари Marvel. Каратель. Том 1</t>
+          <t>Истории монстров. Том 1.</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>1200</v>
+        <v>355</v>
       </c>
       <c r="D242" t="inlineStr">
         <is>
@@ -6004,11 +6004,11 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Последнее путешествие девочек. Том 1</t>
+          <t>Восхождение Героя Щита. Том 12.</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>510</v>
+        <v>315</v>
       </c>
       <c r="D243" t="inlineStr">
         <is>
@@ -6027,7 +6027,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Очень приятно, бог. Том 18.</t>
+          <t>Восхождение Героя Щита. Том 10.</t>
         </is>
       </c>
       <c r="C244" t="n">
@@ -6050,7 +6050,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Очень приятно, бог. Том 17.</t>
+          <t>Восхождение Героя Щита. Том 13.</t>
         </is>
       </c>
       <c r="C245" t="n">
@@ -6073,11 +6073,11 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Очень приятно, бог. Том 16.</t>
+          <t>Тетрадь дружбы Нацумэ. Том 1.</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>315</v>
+        <v>550</v>
       </c>
       <c r="D246" t="inlineStr">
         <is>
@@ -6096,11 +6096,11 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Эмбрион мира. Том 10.</t>
+          <t>Бездомный бог. Том 13.</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>460</v>
+        <v>355</v>
       </c>
       <c r="D247" t="inlineStr">
         <is>
@@ -6119,11 +6119,11 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Мороженщик. Том 1. Радужная обсыпка</t>
+          <t>Sailor Moon. Том 1.</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>470</v>
+        <v>390</v>
       </c>
       <c r="D248" t="inlineStr">
         <is>
@@ -6142,11 +6142,11 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Джузеппе Бергман. Том 1.</t>
+          <t>Бездомный бог. Том 1.</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>795</v>
+        <v>355</v>
       </c>
       <c r="D249" t="inlineStr">
         <is>
@@ -6165,7 +6165,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Нелюдь. Том 10.</t>
+          <t>Ты сияешь лунной ночью. Том 1.</t>
         </is>
       </c>
       <c r="C250" t="n">
@@ -6188,11 +6188,11 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Очень приятно, бог. Том 15.</t>
+          <t>Бездомный бог. Том 15.</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>315</v>
+        <v>355</v>
       </c>
       <c r="D251" t="inlineStr">
         <is>
@@ -6211,11 +6211,11 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Восхождение Героя Щита. Том 13.</t>
+          <t>Восхождение Героя Щита. Том 1.</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>315</v>
+        <v>355</v>
       </c>
       <c r="D252" t="inlineStr">
         <is>
@@ -6234,7 +6234,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Очень приятно, бог. Том 14.</t>
+          <t>У меня мало друзей. Том 17.</t>
         </is>
       </c>
       <c r="C253" t="n">
@@ -6257,11 +6257,11 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Восхождение Героя Щита. Том 12.</t>
+          <t>Врата;Штейна 0. Том 1.</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>315</v>
+        <v>355</v>
       </c>
       <c r="D254" t="inlineStr">
         <is>
@@ -6280,11 +6280,11 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Бдительный Эгути-кун. Том 1</t>
+          <t>Созданный в Бездне. Том 1</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>275</v>
+        <v>360</v>
       </c>
       <c r="D255" t="inlineStr">
         <is>
@@ -6303,11 +6303,11 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Триган. Том 1. Человек на $$60 миллиардов.</t>
+          <t>Очень приятно, бог. Том 16.</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>390</v>
+        <v>315</v>
       </c>
       <c r="D256" t="inlineStr">
         <is>
@@ -6326,11 +6326,11 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Бегущий по лезвию 2019. Том 1</t>
+          <t>Очень приятно, бог. Том 17.</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>470</v>
+        <v>315</v>
       </c>
       <c r="D257" t="inlineStr">
         <is>
@@ -6349,11 +6349,11 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Научное доказательство любви. Том 1.</t>
+          <t>Хвост Феи. Том 10.</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="D258" t="inlineStr">
         <is>
@@ -6372,11 +6372,11 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Хребты Безумия. Том 1 (иллюстр. Ф. Баранже)</t>
+          <t>Очень приятно, бог. Том 18.</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>820</v>
+        <v>315</v>
       </c>
       <c r="D259" t="inlineStr">
         <is>
@@ -6395,11 +6395,11 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Лучшее время жизни. Том 1.</t>
+          <t>Очень приятно, бог. Том 14.</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>580</v>
+        <v>315</v>
       </c>
       <c r="D260" t="inlineStr">
         <is>
@@ -6418,11 +6418,11 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Ангелы смерти. Том 1. Ад приближается</t>
+          <t>«Страна чудес смертников». Том 10.</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>390</v>
+        <v>355</v>
       </c>
       <c r="D261" t="inlineStr">
         <is>
@@ -6441,11 +6441,11 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Горячий парень Джей. Том 1. Вампиры и машины</t>
+          <t>Очень приятно, бог. Том 15.</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>390</v>
+        <v>315</v>
       </c>
       <c r="D262" t="inlineStr">
         <is>
@@ -6464,11 +6464,11 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>У меня мало друзей. Том 17.</t>
+          <t>Без игры жизни нет. Том 1.</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>315</v>
+        <v>355</v>
       </c>
       <c r="D263" t="inlineStr">
         <is>
@@ -6487,11 +6487,11 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Необъятный океан. Том 1.</t>
+          <t>Хвост Феи. Том 12.</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>530</v>
+        <v>365</v>
       </c>
       <c r="D264" t="inlineStr">
         <is>
@@ -6510,11 +6510,11 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Ложные выводы. Том 1</t>
+          <t>Хвост Феи. Том 11.</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>530</v>
+        <v>365</v>
       </c>
       <c r="D265" t="inlineStr">
         <is>
@@ -6533,11 +6533,11 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Сага о Винланде. Том 1</t>
+          <t>Ложные выводы. Том 1</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>865</v>
+        <v>530</v>
       </c>
       <c r="D266" t="inlineStr">
         <is>
@@ -6556,11 +6556,11 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Дабл ми. Том 1.</t>
+          <t>«Страна чудес смертников». Том 1</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="D267" t="inlineStr">
         <is>
@@ -6579,11 +6579,11 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Восхождение Героя Щита. Том 10.</t>
+          <t>Нелюдь. Том 10.</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>315</v>
+        <v>355</v>
       </c>
       <c r="D268" t="inlineStr">
         <is>
@@ -6602,11 +6602,11 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Энциклопедия Dragon Age: Мир Тедаса. Том 1</t>
+          <t>Нелюдь. Том 11.</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>1430</v>
+        <v>355</v>
       </c>
       <c r="D269" t="inlineStr">
         <is>
@@ -6625,11 +6625,11 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Ателье колдовских колпаков. Том 1</t>
+          <t>«Страна чудес смертников». Том 11.</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>450</v>
+        <v>355</v>
       </c>
       <c r="D270" t="inlineStr">
         <is>
@@ -6648,11 +6648,11 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Динозавры в комиксах. Том 1</t>
+          <t>«Страна чудес смертников». Том 12.</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>990</v>
+        <v>355</v>
       </c>
       <c r="D271" t="inlineStr">
         <is>
@@ -6671,11 +6671,11 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Дюрарара!! Том 1</t>
+          <t>«Страна чудес смертников». Том 13.</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>865</v>
+        <v>355</v>
       </c>
       <c r="D272" t="inlineStr">
         <is>
@@ -6694,11 +6694,11 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Твоя апрельская ложь. Том 1</t>
+          <t>У меня мало друзей. Том 1. Ver.1.1 (Исправленное и дополненное издание).</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>450</v>
+        <v>355</v>
       </c>
       <c r="D273" t="inlineStr">
         <is>
@@ -6740,11 +6740,11 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Экслибриум. Жизнь вторая. Том 1. Безвозвратно</t>
+          <t>Хвост Феи. Том 1.</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>475</v>
+        <v>365</v>
       </c>
       <c r="D275" t="inlineStr">
         <is>
@@ -6763,11 +6763,11 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Арчи и Сабрина. Том 1</t>
+          <t>Торадора! Том 1.</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>420</v>
+        <v>255</v>
       </c>
       <c r="D276" t="inlineStr">
         <is>
@@ -6786,11 +6786,11 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Подростки Мутанты Ниндзя Черепашки. Вселенная. Том 1. Грядущая война</t>
+          <t>Очень приятно, бог. Том 10.</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>410</v>
+        <v>315</v>
       </c>
       <c r="D277" t="inlineStr">
         <is>
@@ -6809,11 +6809,11 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Приключения Огурчика. Том 1. Пончиковое королевство</t>
+          <t>Очень приятно, бог. Том 12.</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>865</v>
+        <v>315</v>
       </c>
       <c r="D278" t="inlineStr">
         <is>
@@ -6832,11 +6832,11 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Дневник будущего. Том 12</t>
+          <t>Очень приятно, бог. Том 11.</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="D279" t="inlineStr">
         <is>
@@ -6855,11 +6855,11 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Эльф не может похудеть. Том 1</t>
+          <t>Необъятный океан. Том 1.</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>340</v>
+        <v>530</v>
       </c>
       <c r="D280" t="inlineStr">
         <is>
@@ -6878,11 +6878,11 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Блюз мачехи и дочери. Том 1.</t>
+          <t>Blame! Том 10.</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="D281" t="inlineStr">
         <is>
@@ -6901,7 +6901,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Ты сияешь лунной ночью. Том 1.</t>
+          <t>Врата;Штейна. Том 1</t>
         </is>
       </c>
       <c r="C282" t="n">
@@ -6924,11 +6924,11 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Магазинчик обуви. Том 1.</t>
+          <t>Хвост Феи. Том 13.</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>390</v>
+        <v>365</v>
       </c>
       <c r="D283" t="inlineStr">
         <is>
@@ -6947,11 +6947,11 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Лаура-разбойница: юные девы, рыцари, заговорщики. Том 1.</t>
+          <t>Последнее путешествие девочек. Том 1</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>970</v>
+        <v>510</v>
       </c>
       <c r="D284" t="inlineStr">
         <is>
@@ -6970,11 +6970,11 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Хвост Феи. Том 12.</t>
+          <t>Научное доказательство любви. Том 1.</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="D285" t="inlineStr">
         <is>
@@ -6993,11 +6993,11 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Хвост Феи. Том 11.</t>
+          <t>GUNNM. Том 1.</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="D286" t="inlineStr">
         <is>
@@ -7016,7 +7016,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Чудовище за соседней партой. Том 13.</t>
+          <t>Blame! Том 1.</t>
         </is>
       </c>
       <c r="C287" t="n">
@@ -7039,7 +7039,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Чудовище за соседней партой. Том 12.</t>
+          <t>Чудовище за соседней партой. Том 11.</t>
         </is>
       </c>
       <c r="C288" t="n">
@@ -7062,11 +7062,11 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Чудовище за соседней партой. Том 11.</t>
+          <t>Эльф не может похудеть. Том 1</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>315</v>
+        <v>340</v>
       </c>
       <c r="D289" t="inlineStr">
         <is>
@@ -7085,11 +7085,11 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Академия Мстителей. Том 1</t>
+          <t>Чудовище за соседней партой. Том 12.</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>1065</v>
+        <v>315</v>
       </c>
       <c r="D290" t="inlineStr">
         <is>
@@ -7108,11 +7108,11 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Семь смертных грехов. Том 1.</t>
+          <t>Паразит. Том 1.</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>550</v>
+        <v>495</v>
       </c>
       <c r="D291" t="inlineStr">
         <is>
@@ -7131,11 +7131,11 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Дневник будущего. Том 10</t>
+          <t>Чудовище за соседней партой. Том 13.</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="D292" t="inlineStr">
         <is>
@@ -7154,11 +7154,11 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Ария. Том 1.</t>
+          <t>Я - Сакамото, а что? Том 1.</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>645</v>
+        <v>355</v>
       </c>
       <c r="D293" t="inlineStr">
         <is>
@@ -7177,11 +7177,11 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Хвост Феи. Том 10.</t>
+          <t>У меня мало друзей. Том 14.</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>365</v>
+        <v>300</v>
       </c>
       <c r="D294" t="inlineStr">
         <is>
@@ -7200,11 +7200,11 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Истории монстров. Том 1.</t>
+          <t>У меня мало друзей. Том 15.</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="D295" t="inlineStr">
         <is>
@@ -7223,11 +7223,11 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Новая Росомаха. Том 1</t>
+          <t>Ария. Том 1.</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>585</v>
+        <v>645</v>
       </c>
       <c r="D296" t="inlineStr">
         <is>
@@ -7246,11 +7246,11 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Роскошный карат. Добродетель тьмы. Том 1.</t>
+          <t>Город кислоты. Том 1. Ver.1.1 (Исправленное и дополненное издание).</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="D297" t="inlineStr">
         <is>
@@ -7269,7 +7269,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Очень приятно, бог. Том 12.</t>
+          <t>У меня мало друзей. Том 16.</t>
         </is>
       </c>
       <c r="C298" t="n">
@@ -7292,11 +7292,11 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Очень приятно, бог. Том 11.</t>
+          <t>У меня мало друзей. Том 13.</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>315</v>
+        <v>260</v>
       </c>
       <c r="D299" t="inlineStr">
         <is>
@@ -7315,7 +7315,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Интриги Ватсона и новый Шерлок Холмс. Том 1</t>
+          <t>Бдительный Эгути-кун. Том 1</t>
         </is>
       </c>
       <c r="C300" t="n">
@@ -7338,11 +7338,11 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Очень приятно, бог. Том 10.</t>
+          <t>Дневник будущего. Том 12</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="D301" t="inlineStr">
         <is>
@@ -7361,11 +7361,11 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>За гранью времен Г. Ф. Лавкрафта. Том 1</t>
+          <t>У меня мало друзей. Том 12.</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>370</v>
+        <v>260</v>
       </c>
       <c r="D302" t="inlineStr">
         <is>
@@ -7384,11 +7384,11 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Фиолетовое поле Лариона. Том 1</t>
+          <t>У меня мало друзей. Том 10.</t>
         </is>
       </c>
       <c r="C303" t="n">
-        <v>400</v>
+        <v>260</v>
       </c>
       <c r="D303" t="inlineStr">
         <is>
@@ -7407,11 +7407,11 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Чудовище за соседней партой. Том 10.</t>
+          <t>У меня мало друзей. Том 11.</t>
         </is>
       </c>
       <c r="C304" t="n">
-        <v>315</v>
+        <v>260</v>
       </c>
       <c r="D304" t="inlineStr">
         <is>
@@ -7430,11 +7430,11 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Метабарон. Том 1 (Выпуски 1-4)</t>
+          <t>Скитания Эманон. Том 1.</t>
         </is>
       </c>
       <c r="C305" t="n">
-        <v>995</v>
+        <v>390</v>
       </c>
       <c r="D305" t="inlineStr">
         <is>
@@ -7453,11 +7453,11 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Дракорничная госпожи Кобаяси. Том 1</t>
+          <t>Чудовище за соседней партой. Том 10.</t>
         </is>
       </c>
       <c r="C306" t="n">
-        <v>450</v>
+        <v>315</v>
       </c>
       <c r="D306" t="inlineStr">
         <is>
@@ -7476,11 +7476,11 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Паразит. Том 1.</t>
+          <t>Дневник будущего. Том 10</t>
         </is>
       </c>
       <c r="C307" t="n">
-        <v>495</v>
+        <v>335</v>
       </c>
       <c r="D307" t="inlineStr">
         <is>
@@ -7499,7 +7499,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Врата;Штейна 0. Том 1.</t>
+          <t>Нелюдь. Том 1.</t>
         </is>
       </c>
       <c r="C308" t="n">
@@ -7522,11 +7522,11 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Блаблабла. Том 1.</t>
+          <t>Чудовище за соседней партой. Том 1.</t>
         </is>
       </c>
       <c r="C309" t="n">
-        <v>450</v>
+        <v>355</v>
       </c>
       <c r="D309" t="inlineStr">
         <is>
@@ -7545,11 +7545,11 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>StarCraft: Линия фронта. Том 1</t>
+          <t>Рыцари «Сидонии». Том 1.</t>
         </is>
       </c>
       <c r="C310" t="n">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="D310" t="inlineStr">
         <is>
@@ -7568,11 +7568,11 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Куклы. Том 12.</t>
+          <t>Стальной Алхимик. Книга 11</t>
         </is>
       </c>
       <c r="C311" t="n">
-        <v>280</v>
+        <v>719</v>
       </c>
       <c r="D311" t="inlineStr">
         <is>
@@ -7591,11 +7591,11 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Неваляшка. Том 1</t>
+          <t>Загадка Дьявола. Том 1.</t>
         </is>
       </c>
       <c r="C312" t="n">
-        <v>450</v>
+        <v>355</v>
       </c>
       <c r="D312" t="inlineStr">
         <is>
@@ -7614,11 +7614,11 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Ванильная глазурь. Том 1.</t>
+          <t>Хвост Феи. Том 14.</t>
         </is>
       </c>
       <c r="C313" t="n">
-        <v>305</v>
+        <v>365</v>
       </c>
       <c r="D313" t="inlineStr">
         <is>
@@ -7637,11 +7637,11 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Новый Человек-Паук 2099. Том 1: Бросок в будущее</t>
+          <t>Тетрадь Смерти: Black Edition. Книга 1</t>
         </is>
       </c>
       <c r="C314" t="n">
-        <v>660</v>
+        <v>805</v>
       </c>
       <c r="D314" t="inlineStr">
         <is>
@@ -7660,11 +7660,11 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Майлз Моралес: Современный Человек-Паук. Том 1 (Альтернативная обложка)</t>
+          <t>Нахальный принц и кошка-несмеяна. Том 1. Ver.1.1 (Исправленное и дополненное издание).</t>
         </is>
       </c>
       <c r="C315" t="n">
-        <v>800</v>
+        <v>355</v>
       </c>
       <c r="D315" t="inlineStr">
         <is>
@@ -7683,11 +7683,11 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Мстители. Время на исходе. Том 1</t>
+          <t>All You Need Is Kill. Грань будущего. Том 1.</t>
         </is>
       </c>
       <c r="C316" t="n">
-        <v>550</v>
+        <v>420</v>
       </c>
       <c r="D316" t="inlineStr">
         <is>
@@ -7706,11 +7706,11 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>У меня мало друзей. Том 16.</t>
+          <t>Странники. Том 1.</t>
         </is>
       </c>
       <c r="C317" t="n">
-        <v>315</v>
+        <v>470</v>
       </c>
       <c r="D317" t="inlineStr">
         <is>
@@ -7729,11 +7729,11 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Время приключений. Избранное. Том 1</t>
+          <t>Аква. Том 1.</t>
         </is>
       </c>
       <c r="C318" t="n">
-        <v>980</v>
+        <v>280</v>
       </c>
       <c r="D318" t="inlineStr">
         <is>
@@ -7752,11 +7752,11 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Пророк. Том 1.</t>
+          <t>Бакуман. Книга 1</t>
         </is>
       </c>
       <c r="C319" t="n">
-        <v>585</v>
+        <v>539</v>
       </c>
       <c r="D319" t="inlineStr">
         <is>
@@ -7775,11 +7775,11 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Игорь Угорь. Том 1. (Новая обложка)</t>
+          <t>Дабл ми. Том 1.</t>
         </is>
       </c>
       <c r="C320" t="n">
-        <v>160</v>
+        <v>335</v>
       </c>
       <c r="D320" t="inlineStr">
         <is>
@@ -7798,11 +7798,11 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Дракон в поисках дома. Том 1</t>
+          <t>Милый дом Чи. Книга 1</t>
         </is>
       </c>
       <c r="C321" t="n">
-        <v>450</v>
+        <v>305</v>
       </c>
       <c r="D321" t="inlineStr">
         <is>
@@ -7810,3387 +7810,6 @@
         </is>
       </c>
       <c r="E321" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="322">
-      <c r="A322" s="1" t="n">
-        <v>320</v>
-      </c>
-      <c r="B322" t="inlineStr">
-        <is>
-          <t>Капитан Марвел. Том 1. Выше, дальше, быстрее, больше</t>
-        </is>
-      </c>
-      <c r="C322" t="n">
-        <v>400</v>
-      </c>
-      <c r="D322" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E322" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="323">
-      <c r="A323" s="1" t="n">
-        <v>321</v>
-      </c>
-      <c r="B323" t="inlineStr">
-        <is>
-          <t>Нелюбимый. Том 13.</t>
-        </is>
-      </c>
-      <c r="C323" t="n">
-        <v>400</v>
-      </c>
-      <c r="D323" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E323" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="324">
-      <c r="A324" s="1" t="n">
-        <v>322</v>
-      </c>
-      <c r="B324" t="inlineStr">
-        <is>
-          <t>Sword Art Online. Том 14. Алисизация. Единство</t>
-        </is>
-      </c>
-      <c r="C324" t="n">
-        <v>810</v>
-      </c>
-      <c r="D324" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E324" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="325">
-      <c r="A325" s="1" t="n">
-        <v>323</v>
-      </c>
-      <c r="B325" t="inlineStr">
-        <is>
-          <t>Странные дела. Том 1</t>
-        </is>
-      </c>
-      <c r="C325" t="n">
-        <v>450</v>
-      </c>
-      <c r="D325" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E325" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="326">
-      <c r="A326" s="1" t="n">
-        <v>324</v>
-      </c>
-      <c r="B326" t="inlineStr">
-        <is>
-          <t>Манман-тян, ан! Священные узы. Том 1.</t>
-        </is>
-      </c>
-      <c r="C326" t="n">
-        <v>275</v>
-      </c>
-      <c r="D326" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E326" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="327">
-      <c r="A327" s="1" t="n">
-        <v>325</v>
-      </c>
-      <c r="B327" t="inlineStr">
-        <is>
-          <t>Созданный в Бездне. Том 1</t>
-        </is>
-      </c>
-      <c r="C327" t="n">
-        <v>360</v>
-      </c>
-      <c r="D327" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E327" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="328">
-      <c r="A328" s="1" t="n">
-        <v>326</v>
-      </c>
-      <c r="B328" t="inlineStr">
-        <is>
-          <t>Пять миров. Том 1. Воин песка</t>
-        </is>
-      </c>
-      <c r="C328" t="n">
-        <v>760</v>
-      </c>
-      <c r="D328" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E328" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="329">
-      <c r="A329" s="1" t="n">
-        <v>327</v>
-      </c>
-      <c r="B329" t="inlineStr">
-        <is>
-          <t>Мстители. Том 1. Мир Мстителей.</t>
-        </is>
-      </c>
-      <c r="C329" t="n">
-        <v>390</v>
-      </c>
-      <c r="D329" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E329" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="330">
-      <c r="A330" s="1" t="n">
-        <v>328</v>
-      </c>
-      <c r="B330" t="inlineStr">
-        <is>
-          <t>Странная жизнь Субару. Том 1</t>
-        </is>
-      </c>
-      <c r="C330" t="n">
-        <v>280</v>
-      </c>
-      <c r="D330" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E330" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="331">
-      <c r="A331" s="1" t="n">
-        <v>329</v>
-      </c>
-      <c r="B331" t="inlineStr">
-        <is>
-          <t>«Страна чудес смертников». Том 1</t>
-        </is>
-      </c>
-      <c r="C331" t="n">
-        <v>355</v>
-      </c>
-      <c r="D331" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E331" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="332">
-      <c r="A332" s="1" t="n">
-        <v>330</v>
-      </c>
-      <c r="B332" t="inlineStr">
-        <is>
-          <t>Хвост Феи. Том 1.</t>
-        </is>
-      </c>
-      <c r="C332" t="n">
-        <v>365</v>
-      </c>
-      <c r="D332" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E332" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="333">
-      <c r="A333" s="1" t="n">
-        <v>331</v>
-      </c>
-      <c r="B333" t="inlineStr">
-        <is>
-          <t>Путешествие к центру земли. Том 1.</t>
-        </is>
-      </c>
-      <c r="C333" t="n">
-        <v>430</v>
-      </c>
-      <c r="D333" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E333" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="334">
-      <c r="A334" s="1" t="n">
-        <v>332</v>
-      </c>
-      <c r="B334" t="inlineStr">
-        <is>
-          <t>Симпсоны. Антология. Том 1</t>
-        </is>
-      </c>
-      <c r="C334" t="n">
-        <v>400</v>
-      </c>
-      <c r="D334" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E334" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="335">
-      <c r="A335" s="1" t="n">
-        <v>333</v>
-      </c>
-      <c r="B335" t="inlineStr">
-        <is>
-          <t>Номер один. Том 18.</t>
-        </is>
-      </c>
-      <c r="C335" t="n">
-        <v>280</v>
-      </c>
-      <c r="D335" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E335" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="336">
-      <c r="A336" s="1" t="n">
-        <v>334</v>
-      </c>
-      <c r="B336" t="inlineStr">
-        <is>
-          <t>Хребты безумия Г. Ф. Лавкрафта. Том 1</t>
-        </is>
-      </c>
-      <c r="C336" t="n">
-        <v>370</v>
-      </c>
-      <c r="D336" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E336" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="337">
-      <c r="A337" s="1" t="n">
-        <v>335</v>
-      </c>
-      <c r="B337" t="inlineStr">
-        <is>
-          <t>Ольга, девочка из цирка. Том 1</t>
-        </is>
-      </c>
-      <c r="C337" t="n">
-        <v>335</v>
-      </c>
-      <c r="D337" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E337" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="338">
-      <c r="A338" s="1" t="n">
-        <v>336</v>
-      </c>
-      <c r="B338" t="inlineStr">
-        <is>
-          <t>Новые Мстители. Том 1. Всё умирает.</t>
-        </is>
-      </c>
-      <c r="C338" t="n">
-        <v>390</v>
-      </c>
-      <c r="D338" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E338" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="339">
-      <c r="A339" s="1" t="n">
-        <v>337</v>
-      </c>
-      <c r="B339" t="inlineStr">
-        <is>
-          <t>Детектив Энола Холмс. Том 1. Двойное исчезновение</t>
-        </is>
-      </c>
-      <c r="C339" t="n">
-        <v>765</v>
-      </c>
-      <c r="D339" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E339" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="340">
-      <c r="A340" s="1" t="n">
-        <v>338</v>
-      </c>
-      <c r="B340" t="inlineStr">
-        <is>
-          <t>Она — Монстр. Том 1. Пробуждение</t>
-        </is>
-      </c>
-      <c r="C340" t="n">
-        <v>480</v>
-      </c>
-      <c r="D340" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E340" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="341">
-      <c r="A341" s="1" t="n">
-        <v>339</v>
-      </c>
-      <c r="B341" t="inlineStr">
-        <is>
-          <t>Номер один. Том 17.</t>
-        </is>
-      </c>
-      <c r="C341" t="n">
-        <v>280</v>
-      </c>
-      <c r="D341" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E341" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="342">
-      <c r="A342" s="1" t="n">
-        <v>340</v>
-      </c>
-      <c r="B342" t="inlineStr">
-        <is>
-          <t>Номер один. Том 16.</t>
-        </is>
-      </c>
-      <c r="C342" t="n">
-        <v>280</v>
-      </c>
-      <c r="D342" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E342" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="343">
-      <c r="A343" s="1" t="n">
-        <v>341</v>
-      </c>
-      <c r="B343" t="inlineStr">
-        <is>
-          <t>Sailor Moon. Том 1.</t>
-        </is>
-      </c>
-      <c r="C343" t="n">
-        <v>390</v>
-      </c>
-      <c r="D343" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E343" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="344">
-      <c r="A344" s="1" t="n">
-        <v>342</v>
-      </c>
-      <c r="B344" t="inlineStr">
-        <is>
-          <t>Blame! Том 10.</t>
-        </is>
-      </c>
-      <c r="C344" t="n">
-        <v>315</v>
-      </c>
-      <c r="D344" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E344" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="345">
-      <c r="A345" s="1" t="n">
-        <v>343</v>
-      </c>
-      <c r="B345" t="inlineStr">
-        <is>
-          <t>The Boys: Пацаны. Том 1. Самое главное</t>
-        </is>
-      </c>
-      <c r="C345" t="n">
-        <v>520</v>
-      </c>
-      <c r="D345" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E345" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="346">
-      <c r="A346" s="1" t="n">
-        <v>344</v>
-      </c>
-      <c r="B346" t="inlineStr">
-        <is>
-          <t>Город, в котором меня нет. Том 1</t>
-        </is>
-      </c>
-      <c r="C346" t="n">
-        <v>450</v>
-      </c>
-      <c r="D346" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E346" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="347">
-      <c r="A347" s="1" t="n">
-        <v>345</v>
-      </c>
-      <c r="B347" t="inlineStr">
-        <is>
-          <t>Странники. Том 1.</t>
-        </is>
-      </c>
-      <c r="C347" t="n">
-        <v>470</v>
-      </c>
-      <c r="D347" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E347" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="348">
-      <c r="A348" s="1" t="n">
-        <v>346</v>
-      </c>
-      <c r="B348" t="inlineStr">
-        <is>
-          <t>Человек-Паук 2099. Том 1. Вне времени. (Новая обложка)</t>
-        </is>
-      </c>
-      <c r="C348" t="n">
-        <v>400</v>
-      </c>
-      <c r="D348" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E348" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="349">
-      <c r="A349" s="1" t="n">
-        <v>347</v>
-      </c>
-      <c r="B349" t="inlineStr">
-        <is>
-          <t>Номер один. Том 15.</t>
-        </is>
-      </c>
-      <c r="C349" t="n">
-        <v>280</v>
-      </c>
-      <c r="D349" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E349" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="350">
-      <c r="A350" s="1" t="n">
-        <v>348</v>
-      </c>
-      <c r="B350" t="inlineStr">
-        <is>
-          <t>Росомаха. Старик Логан. Полное издание. Том 1</t>
-        </is>
-      </c>
-      <c r="C350" t="n">
-        <v>505</v>
-      </c>
-      <c r="D350" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E350" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="351">
-      <c r="A351" s="1" t="n">
-        <v>349</v>
-      </c>
-      <c r="B351" t="inlineStr">
-        <is>
-          <t>Графство Эссекс. Том 1. Жизнь на ферме.</t>
-        </is>
-      </c>
-      <c r="C351" t="n">
-        <v>395</v>
-      </c>
-      <c r="D351" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E351" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="352">
-      <c r="A352" s="1" t="n">
-        <v>350</v>
-      </c>
-      <c r="B352" t="inlineStr">
-        <is>
-          <t>Куклы. Том 11.</t>
-        </is>
-      </c>
-      <c r="C352" t="n">
-        <v>280</v>
-      </c>
-      <c r="D352" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E352" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="353">
-      <c r="A353" s="1" t="n">
-        <v>351</v>
-      </c>
-      <c r="B353" t="inlineStr">
-        <is>
-          <t>Загадка Дьявола. Том 1.</t>
-        </is>
-      </c>
-      <c r="C353" t="n">
-        <v>355</v>
-      </c>
-      <c r="D353" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E353" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="354">
-      <c r="A354" s="1" t="n">
-        <v>352</v>
-      </c>
-      <c r="B354" t="inlineStr">
-        <is>
-          <t>Джагхед. Том 1</t>
-        </is>
-      </c>
-      <c r="C354" t="n">
-        <v>470</v>
-      </c>
-      <c r="D354" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E354" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="355">
-      <c r="A355" s="1" t="n">
-        <v>353</v>
-      </c>
-      <c r="B355" t="inlineStr">
-        <is>
-          <t>Номер один. Том 14.</t>
-        </is>
-      </c>
-      <c r="C355" t="n">
-        <v>280</v>
-      </c>
-      <c r="D355" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E355" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="356">
-      <c r="A356" s="1" t="n">
-        <v>354</v>
-      </c>
-      <c r="B356" t="inlineStr">
-        <is>
-          <t>Нелюбимый. Том 12.</t>
-        </is>
-      </c>
-      <c r="C356" t="n">
-        <v>400</v>
-      </c>
-      <c r="D356" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E356" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="357">
-      <c r="A357" s="1" t="n">
-        <v>355</v>
-      </c>
-      <c r="B357" t="inlineStr">
-        <is>
-          <t>Warcraft: Легенды. Том 1</t>
-        </is>
-      </c>
-      <c r="C357" t="n">
-        <v>340</v>
-      </c>
-      <c r="D357" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E357" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="358">
-      <c r="A358" s="1" t="n">
-        <v>356</v>
-      </c>
-      <c r="B358" t="inlineStr">
-        <is>
-          <t>Номер один. Том 13.</t>
-        </is>
-      </c>
-      <c r="C358" t="n">
-        <v>280</v>
-      </c>
-      <c r="D358" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E358" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="359">
-      <c r="A359" s="1" t="n">
-        <v>357</v>
-      </c>
-      <c r="B359" t="inlineStr">
-        <is>
-          <t>Время Приключений. Полное издание. Том 1</t>
-        </is>
-      </c>
-      <c r="C359" t="n">
-        <v>1015</v>
-      </c>
-      <c r="D359" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E359" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="360">
-      <c r="A360" s="1" t="n">
-        <v>358</v>
-      </c>
-      <c r="B360" t="inlineStr">
-        <is>
-          <t>Ниндзяк. Том 1. Оружейник</t>
-        </is>
-      </c>
-      <c r="C360" t="n">
-        <v>430</v>
-      </c>
-      <c r="D360" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E360" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="361">
-      <c r="A361" s="1" t="n">
-        <v>359</v>
-      </c>
-      <c r="B361" t="inlineStr">
-        <is>
-          <t>Бладшот. Том 1. Подрывая мир</t>
-        </is>
-      </c>
-      <c r="C361" t="n">
-        <v>430</v>
-      </c>
-      <c r="D361" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E361" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="362">
-      <c r="A362" s="1" t="n">
-        <v>360</v>
-      </c>
-      <c r="B362" t="inlineStr">
-        <is>
-          <t>GUNNM. Том 1.</t>
-        </is>
-      </c>
-      <c r="C362" t="n">
-        <v>375</v>
-      </c>
-      <c r="D362" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E362" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="363">
-      <c r="A363" s="1" t="n">
-        <v>361</v>
-      </c>
-      <c r="B363" t="inlineStr">
-        <is>
-          <t>Нелюбимый. Том 11.</t>
-        </is>
-      </c>
-      <c r="C363" t="n">
-        <v>335</v>
-      </c>
-      <c r="D363" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E363" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="364">
-      <c r="A364" s="1" t="n">
-        <v>362</v>
-      </c>
-      <c r="B364" t="inlineStr">
-        <is>
-          <t>Гарфилд. Том 1</t>
-        </is>
-      </c>
-      <c r="C364" t="n">
-        <v>550</v>
-      </c>
-      <c r="D364" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E364" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="365">
-      <c r="A365" s="1" t="n">
-        <v>363</v>
-      </c>
-      <c r="B365" t="inlineStr">
-        <is>
-          <t>У меня мало друзей. Том 15.</t>
-        </is>
-      </c>
-      <c r="C365" t="n">
-        <v>315</v>
-      </c>
-      <c r="D365" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E365" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="366">
-      <c r="A366" s="1" t="n">
-        <v>364</v>
-      </c>
-      <c r="B366" t="inlineStr">
-        <is>
-          <t>Бандак. Том 1</t>
-        </is>
-      </c>
-      <c r="C366" t="n">
-        <v>370</v>
-      </c>
-      <c r="D366" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E366" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="367">
-      <c r="A367" s="1" t="n">
-        <v>365</v>
-      </c>
-      <c r="B367" t="inlineStr">
-        <is>
-          <t>Куклы. Том 10.</t>
-        </is>
-      </c>
-      <c r="C367" t="n">
-        <v>280</v>
-      </c>
-      <c r="D367" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E367" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="368">
-      <c r="A368" s="1" t="n">
-        <v>366</v>
-      </c>
-      <c r="B368" t="inlineStr">
-        <is>
-          <t>Саша и Томкруз Том 1. У викингов</t>
-        </is>
-      </c>
-      <c r="C368" t="n">
-        <v>705</v>
-      </c>
-      <c r="D368" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E368" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="369">
-      <c r="A369" s="1" t="n">
-        <v>367</v>
-      </c>
-      <c r="B369" t="inlineStr">
-        <is>
-          <t>Таймасин. Дневник экзорциста. Том 1</t>
-        </is>
-      </c>
-      <c r="C369" t="n">
-        <v>400</v>
-      </c>
-      <c r="D369" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E369" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="370">
-      <c r="A370" s="1" t="n">
-        <v>368</v>
-      </c>
-      <c r="B370" t="inlineStr">
-        <is>
-          <t>Нелюбимый. Том 10.</t>
-        </is>
-      </c>
-      <c r="C370" t="n">
-        <v>335</v>
-      </c>
-      <c r="D370" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E370" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="371">
-      <c r="A371" s="1" t="n">
-        <v>369</v>
-      </c>
-      <c r="B371" t="inlineStr">
-        <is>
-          <t>Sword Art Online. Том 10. Алисизация. Запуск</t>
-        </is>
-      </c>
-      <c r="C371" t="n">
-        <v>810</v>
-      </c>
-      <c r="D371" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E371" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="372">
-      <c r="A372" s="1" t="n">
-        <v>370</v>
-      </c>
-      <c r="B372" t="inlineStr">
-        <is>
-          <t>Sword Art Online: Progressive. Том 1</t>
-        </is>
-      </c>
-      <c r="C372" t="n">
-        <v>810</v>
-      </c>
-      <c r="D372" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E372" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="373">
-      <c r="A373" s="1" t="n">
-        <v>371</v>
-      </c>
-      <c r="B373" t="inlineStr">
-        <is>
-          <t>Re:Zero. Жизнь с нуля в альтернативном мире. День в столице королевства. Том 1</t>
-        </is>
-      </c>
-      <c r="C373" t="n">
-        <v>450</v>
-      </c>
-      <c r="D373" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E373" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="374">
-      <c r="A374" s="1" t="n">
-        <v>372</v>
-      </c>
-      <c r="B374" t="inlineStr">
-        <is>
-          <t>Overlord. Том 1. Король-нежить</t>
-        </is>
-      </c>
-      <c r="C374" t="n">
-        <v>810</v>
-      </c>
-      <c r="D374" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E374" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="375">
-      <c r="A375" s="1" t="n">
-        <v>373</v>
-      </c>
-      <c r="B375" t="inlineStr">
-        <is>
-          <t>Атлас и Аксис. Том 1.</t>
-        </is>
-      </c>
-      <c r="C375" t="n">
-        <v>550</v>
-      </c>
-      <c r="D375" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E375" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="376">
-      <c r="A376" s="1" t="n">
-        <v>374</v>
-      </c>
-      <c r="B376" t="inlineStr">
-        <is>
-          <t>Overwatch: Антология. Том 1</t>
-        </is>
-      </c>
-      <c r="C376" t="n">
-        <v>700</v>
-      </c>
-      <c r="D376" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E376" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="377">
-      <c r="A377" s="1" t="n">
-        <v>375</v>
-      </c>
-      <c r="B377" t="inlineStr">
-        <is>
-          <t>Джек Фрост. Том 11.</t>
-        </is>
-      </c>
-      <c r="C377" t="n">
-        <v>280</v>
-      </c>
-      <c r="D377" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E377" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="378">
-      <c r="A378" s="1" t="n">
-        <v>376</v>
-      </c>
-      <c r="B378" t="inlineStr">
-        <is>
-          <t>Рыцари «Сидонии». Том 1.</t>
-        </is>
-      </c>
-      <c r="C378" t="n">
-        <v>300</v>
-      </c>
-      <c r="D378" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E378" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="379">
-      <c r="A379" s="1" t="n">
-        <v>377</v>
-      </c>
-      <c r="B379" t="inlineStr">
-        <is>
-          <t>Щ.И.Т. Том 1. Идеальная обойма (твердый переплет)</t>
-        </is>
-      </c>
-      <c r="C379" t="n">
-        <v>540</v>
-      </c>
-      <c r="D379" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E379" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="380">
-      <c r="A380" s="1" t="n">
-        <v>378</v>
-      </c>
-      <c r="B380" t="inlineStr">
-        <is>
-          <t>Щ.И.Т. Том 1. Идеальная обойма (мягкий переплет)</t>
-        </is>
-      </c>
-      <c r="C380" t="n">
-        <v>350</v>
-      </c>
-      <c r="D380" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E380" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="381">
-      <c r="A381" s="1" t="n">
-        <v>379</v>
-      </c>
-      <c r="B381" t="inlineStr">
-        <is>
-          <t>Человек-Паук против Зловещей Шестерки. Том 1 (твердая обложка)</t>
-        </is>
-      </c>
-      <c r="C381" t="n">
-        <v>450</v>
-      </c>
-      <c r="D381" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E381" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="382">
-      <c r="A382" s="1" t="n">
-        <v>380</v>
-      </c>
-      <c r="B382" t="inlineStr">
-        <is>
-          <t>Человек-Паук против Зловещей Шестерки. Том 1 (мягкая обложка)</t>
-        </is>
-      </c>
-      <c r="C382" t="n">
-        <v>330</v>
-      </c>
-      <c r="D382" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E382" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="383">
-      <c r="A383" s="1" t="n">
-        <v>381</v>
-      </c>
-      <c r="B383" t="inlineStr">
-        <is>
-          <t>Предвестник. Восход Омеги. Том 1.</t>
-        </is>
-      </c>
-      <c r="C383" t="n">
-        <v>360</v>
-      </c>
-      <c r="D383" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E383" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="384">
-      <c r="A384" s="1" t="n">
-        <v>382</v>
-      </c>
-      <c r="B384" t="inlineStr">
-        <is>
-          <t>Нелюдь. Том 1.</t>
-        </is>
-      </c>
-      <c r="C384" t="n">
-        <v>355</v>
-      </c>
-      <c r="D384" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E384" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="385">
-      <c r="A385" s="1" t="n">
-        <v>383</v>
-      </c>
-      <c r="B385" t="inlineStr">
-        <is>
-          <t>Локи. Агент Асгарда. Том 1. Доверьтесь мне</t>
-        </is>
-      </c>
-      <c r="C385" t="n">
-        <v>385</v>
-      </c>
-      <c r="D385" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E385" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="386">
-      <c r="A386" s="1" t="n">
-        <v>384</v>
-      </c>
-      <c r="B386" t="inlineStr">
-        <is>
-          <t>Порочные + Божества. Том 1. В духе Фауста</t>
-        </is>
-      </c>
-      <c r="C386" t="n">
-        <v>400</v>
-      </c>
-      <c r="D386" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E386" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="387">
-      <c r="A387" s="1" t="n">
-        <v>385</v>
-      </c>
-      <c r="B387" t="inlineStr">
-        <is>
-          <t>Магнето. Том 1. Дурная Слава.</t>
-        </is>
-      </c>
-      <c r="C387" t="n">
-        <v>360</v>
-      </c>
-      <c r="D387" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E387" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="388">
-      <c r="A388" s="1" t="n">
-        <v>386</v>
-      </c>
-      <c r="B388" t="inlineStr">
-        <is>
-          <t>Ну не может моя сестренка быть такой милой. Том 1.</t>
-        </is>
-      </c>
-      <c r="C388" t="n">
-        <v>355</v>
-      </c>
-      <c r="D388" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E388" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="389">
-      <c r="A389" s="1" t="n">
-        <v>387</v>
-      </c>
-      <c r="B389" t="inlineStr">
-        <is>
-          <t>Смурфы. Том 1. Черные смурфы.</t>
-        </is>
-      </c>
-      <c r="C389" t="n">
-        <v>490</v>
-      </c>
-      <c r="D389" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E389" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="390">
-      <c r="A390" s="1" t="n">
-        <v>388</v>
-      </c>
-      <c r="B390" t="inlineStr">
-        <is>
-          <t>Джек Фрост. Том 10.</t>
-        </is>
-      </c>
-      <c r="C390" t="n">
-        <v>280</v>
-      </c>
-      <c r="D390" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E390" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="391">
-      <c r="A391" s="1" t="n">
-        <v>389</v>
-      </c>
-      <c r="B391" t="inlineStr">
-        <is>
-          <t>Дневники Вишенки. Том 1. Каменный зоопарк.</t>
-        </is>
-      </c>
-      <c r="C391" t="n">
-        <v>855</v>
-      </c>
-      <c r="D391" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E391" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="392">
-      <c r="A392" s="1" t="n">
-        <v>390</v>
-      </c>
-      <c r="B392" t="inlineStr">
-        <is>
-          <t>Без игры жизни нет. Том 1.</t>
-        </is>
-      </c>
-      <c r="C392" t="n">
-        <v>430</v>
-      </c>
-      <c r="D392" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E392" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="393">
-      <c r="A393" s="1" t="n">
-        <v>391</v>
-      </c>
-      <c r="B393" t="inlineStr">
-        <is>
-          <t>Звездный замок. 1869: покорение космоса. Том 1</t>
-        </is>
-      </c>
-      <c r="C393" t="n">
-        <v>955</v>
-      </c>
-      <c r="D393" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E393" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="394">
-      <c r="A394" s="1" t="n">
-        <v>392</v>
-      </c>
-      <c r="B394" t="inlineStr">
-        <is>
-          <t>Волчица и пряности. Том 14.</t>
-        </is>
-      </c>
-      <c r="C394" t="n">
-        <v>450</v>
-      </c>
-      <c r="D394" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E394" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="395">
-      <c r="A395" s="1" t="n">
-        <v>393</v>
-      </c>
-      <c r="B395" t="inlineStr">
-        <is>
-          <t>Номер один. Том 12.</t>
-        </is>
-      </c>
-      <c r="C395" t="n">
-        <v>280</v>
-      </c>
-      <c r="D395" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E395" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="396">
-      <c r="A396" s="1" t="n">
-        <v>394</v>
-      </c>
-      <c r="B396" t="inlineStr">
-        <is>
-          <t>Номер один. Том 11.</t>
-        </is>
-      </c>
-      <c r="C396" t="n">
-        <v>280</v>
-      </c>
-      <c r="D396" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E396" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="397">
-      <c r="A397" s="1" t="n">
-        <v>395</v>
-      </c>
-      <c r="B397" t="inlineStr">
-        <is>
-          <t>Человек-Тень. Том 1. Обряды рождения.</t>
-        </is>
-      </c>
-      <c r="C397" t="n">
-        <v>360</v>
-      </c>
-      <c r="D397" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E397" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="398">
-      <c r="A398" s="1" t="n">
-        <v>396</v>
-      </c>
-      <c r="B398" t="inlineStr">
-        <is>
-          <t>У меня мало друзей. Том 14.</t>
-        </is>
-      </c>
-      <c r="C398" t="n">
-        <v>300</v>
-      </c>
-      <c r="D398" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E398" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="399">
-      <c r="A399" s="1" t="n">
-        <v>397</v>
-      </c>
-      <c r="B399" t="inlineStr">
-        <is>
-          <t>Blame! Том 1.</t>
-        </is>
-      </c>
-      <c r="C399" t="n">
-        <v>315</v>
-      </c>
-      <c r="D399" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E399" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="400">
-      <c r="A400" s="1" t="n">
-        <v>398</v>
-      </c>
-      <c r="B400" t="inlineStr">
-        <is>
-          <t>Эххо. Зеркальный мир. Том 1. Нью-Йорк. Парижская империя.</t>
-        </is>
-      </c>
-      <c r="C400" t="n">
-        <v>615</v>
-      </c>
-      <c r="D400" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E400" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="401">
-      <c r="A401" s="1" t="n">
-        <v>399</v>
-      </c>
-      <c r="B401" t="inlineStr">
-        <is>
-          <t>Стражи Галактики. Том 1.</t>
-        </is>
-      </c>
-      <c r="C401" t="n">
-        <v>600</v>
-      </c>
-      <c r="D401" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E401" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="402">
-      <c r="A402" s="1" t="n">
-        <v>400</v>
-      </c>
-      <c r="B402" t="inlineStr">
-        <is>
-          <t>Икс-О Воин. Том 1. Огнем и мечом.</t>
-        </is>
-      </c>
-      <c r="C402" t="n">
-        <v>360</v>
-      </c>
-      <c r="D402" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E402" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="403">
-      <c r="A403" s="1" t="n">
-        <v>401</v>
-      </c>
-      <c r="B403" t="inlineStr">
-        <is>
-          <t>Винни Бартон. Том 1.</t>
-        </is>
-      </c>
-      <c r="C403" t="n">
-        <v>210</v>
-      </c>
-      <c r="D403" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E403" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="404">
-      <c r="A404" s="1" t="n">
-        <v>402</v>
-      </c>
-      <c r="B404" t="inlineStr">
-        <is>
-          <t>Пэтси Уокер, она же Адская кошка! Том 1</t>
-        </is>
-      </c>
-      <c r="C404" t="n">
-        <v>225</v>
-      </c>
-      <c r="D404" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E404" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="405">
-      <c r="A405" s="1" t="n">
-        <v>403</v>
-      </c>
-      <c r="B405" t="inlineStr">
-        <is>
-          <t>Шерлок. Том 1.</t>
-        </is>
-      </c>
-      <c r="C405" t="n">
-        <v>280</v>
-      </c>
-      <c r="D405" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E405" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="406">
-      <c r="A406" s="1" t="n">
-        <v>404</v>
-      </c>
-      <c r="B406" t="inlineStr">
-        <is>
-          <t>Номер один. Том 10.</t>
-        </is>
-      </c>
-      <c r="C406" t="n">
-        <v>280</v>
-      </c>
-      <c r="D406" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E406" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="407">
-      <c r="A407" s="1" t="n">
-        <v>405</v>
-      </c>
-      <c r="B407" t="inlineStr">
-        <is>
-          <t>Star Trek. Том 1.</t>
-        </is>
-      </c>
-      <c r="C407" t="n">
-        <v>370</v>
-      </c>
-      <c r="D407" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E407" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="408">
-      <c r="A408" s="1" t="n">
-        <v>406</v>
-      </c>
-      <c r="B408" t="inlineStr">
-        <is>
-          <t>Кошки-мышки. Старый новый друг. Том 1.</t>
-        </is>
-      </c>
-      <c r="C408" t="n">
-        <v>260</v>
-      </c>
-      <c r="D408" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E408" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="409">
-      <c r="A409" s="1" t="n">
-        <v>407</v>
-      </c>
-      <c r="B409" t="inlineStr">
-        <is>
-          <t>Росомаха и Люди Икс. Том 1.</t>
-        </is>
-      </c>
-      <c r="C409" t="n">
-        <v>415</v>
-      </c>
-      <c r="D409" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E409" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="410">
-      <c r="A410" s="1" t="n">
-        <v>408</v>
-      </c>
-      <c r="B410" t="inlineStr">
-        <is>
-          <t>Джем и Голограммы. Том 1.</t>
-        </is>
-      </c>
-      <c r="C410" t="n">
-        <v>735</v>
-      </c>
-      <c r="D410" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E410" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="411">
-      <c r="A411" s="1" t="n">
-        <v>409</v>
-      </c>
-      <c r="B411" t="inlineStr">
-        <is>
-          <t>Лунная Девочка и ДиноДьявол. Том 1. Лучшие друзья навсегда.</t>
-        </is>
-      </c>
-      <c r="C411" t="n">
-        <v>225</v>
-      </c>
-      <c r="D411" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E411" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="412">
-      <c r="A412" s="1" t="n">
-        <v>410</v>
-      </c>
-      <c r="B412" t="inlineStr">
-        <is>
-          <t>Серебряный Сёрфер. Том 1. Новый рассвет.</t>
-        </is>
-      </c>
-      <c r="C412" t="n">
-        <v>245</v>
-      </c>
-      <c r="D412" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E412" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="413">
-      <c r="A413" s="1" t="n">
-        <v>411</v>
-      </c>
-      <c r="B413" t="inlineStr">
-        <is>
-          <t>Воскресение Рэйчел. Том 1.</t>
-        </is>
-      </c>
-      <c r="C413" t="n">
-        <v>530</v>
-      </c>
-      <c r="D413" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E413" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="414">
-      <c r="A414" s="1" t="n">
-        <v>412</v>
-      </c>
-      <c r="B414" t="inlineStr">
-        <is>
-          <t>Звезда J-pop. Том 1.</t>
-        </is>
-      </c>
-      <c r="C414" t="n">
-        <v>280</v>
-      </c>
-      <c r="D414" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E414" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="415">
-      <c r="A415" s="1" t="n">
-        <v>413</v>
-      </c>
-      <c r="B415" t="inlineStr">
-        <is>
-          <t>One. Том 11</t>
-        </is>
-      </c>
-      <c r="C415" t="n">
-        <v>335</v>
-      </c>
-      <c r="D415" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E415" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="416">
-      <c r="A416" s="1" t="n">
-        <v>414</v>
-      </c>
-      <c r="B416" t="inlineStr">
-        <is>
-          <t>Агенты Щ. И. Т. Том 1. Протоколы Колсона.</t>
-        </is>
-      </c>
-      <c r="C416" t="n">
-        <v>470</v>
-      </c>
-      <c r="D416" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E416" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="417">
-      <c r="A417" s="1" t="n">
-        <v>415</v>
-      </c>
-      <c r="B417" t="inlineStr">
-        <is>
-          <t>Фантастическая Четвёрка. Одни уходят, другие приходят. Том 1.</t>
-        </is>
-      </c>
-      <c r="C417" t="n">
-        <v>390</v>
-      </c>
-      <c r="D417" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E417" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="418">
-      <c r="A418" s="1" t="n">
-        <v>416</v>
-      </c>
-      <c r="B418" t="inlineStr">
-        <is>
-          <t>Электра. Том 1. Кровные узы.</t>
-        </is>
-      </c>
-      <c r="C418" t="n">
-        <v>350</v>
-      </c>
-      <c r="D418" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E418" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="419">
-      <c r="A419" s="1" t="n">
-        <v>417</v>
-      </c>
-      <c r="B419" t="inlineStr">
-        <is>
-          <t>Я - Сакамото, а что? Том 1.</t>
-        </is>
-      </c>
-      <c r="C419" t="n">
-        <v>355</v>
-      </c>
-      <c r="D419" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E419" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="420">
-      <c r="A420" s="1" t="n">
-        <v>418</v>
-      </c>
-      <c r="B420" t="inlineStr">
-        <is>
-          <t>Мисс Марвел. Необычная. Том 1.</t>
-        </is>
-      </c>
-      <c r="C420" t="n">
-        <v>350</v>
-      </c>
-      <c r="D420" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E420" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="421">
-      <c r="A421" s="1" t="n">
-        <v>419</v>
-      </c>
-      <c r="B421" t="inlineStr">
-        <is>
-          <t>One. Том 10</t>
-        </is>
-      </c>
-      <c r="C421" t="n">
-        <v>280</v>
-      </c>
-      <c r="D421" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E421" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="422">
-      <c r="A422" s="1" t="n">
-        <v>420</v>
-      </c>
-      <c r="B422" t="inlineStr">
-        <is>
-          <t>Ведьмы. Том 1.</t>
-        </is>
-      </c>
-      <c r="C422" t="n">
-        <v>585</v>
-      </c>
-      <c r="D422" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E422" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="423">
-      <c r="A423" s="1" t="n">
-        <v>421</v>
-      </c>
-      <c r="B423" t="inlineStr">
-        <is>
-          <t>Силач и Железный Кулак. Том 1. Парни снова в деле.</t>
-        </is>
-      </c>
-      <c r="C423" t="n">
-        <v>350</v>
-      </c>
-      <c r="D423" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E423" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="424">
-      <c r="A424" s="1" t="n">
-        <v>422</v>
-      </c>
-      <c r="B424" t="inlineStr">
-        <is>
-          <t>Железный кулак Том 1: История последнего железного кулака</t>
-        </is>
-      </c>
-      <c r="C424" t="n">
-        <v>375</v>
-      </c>
-      <c r="D424" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E424" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="425">
-      <c r="A425" s="1" t="n">
-        <v>423</v>
-      </c>
-      <c r="B425" t="inlineStr">
-        <is>
-          <t>Фьюри MAX Том 1: Моя война прошла давно</t>
-        </is>
-      </c>
-      <c r="C425" t="n">
-        <v>375</v>
-      </c>
-      <c r="D425" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E425" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="426">
-      <c r="A426" s="1" t="n">
-        <v>424</v>
-      </c>
-      <c r="B426" t="inlineStr">
-        <is>
-          <t>Летние войны. Том 1</t>
-        </is>
-      </c>
-      <c r="C426" t="n">
-        <v>450</v>
-      </c>
-      <c r="D426" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E426" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="427">
-      <c r="A427" s="1" t="n">
-        <v>425</v>
-      </c>
-      <c r="B427" t="inlineStr">
-        <is>
-          <t>My Little Pony. Дружба — это чудо. Том 1.</t>
-        </is>
-      </c>
-      <c r="C427" t="n">
-        <v>550</v>
-      </c>
-      <c r="D427" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E427" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="428">
-      <c r="A428" s="1" t="n">
-        <v>426</v>
-      </c>
-      <c r="B428" t="inlineStr">
-        <is>
-          <t>Призрак в ночи. Том 1</t>
-        </is>
-      </c>
-      <c r="C428" t="n">
-        <v>430</v>
-      </c>
-      <c r="D428" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E428" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="429">
-      <c r="A429" s="1" t="n">
-        <v>427</v>
-      </c>
-      <c r="B429" t="inlineStr">
-        <is>
-          <t>Легенда о Лемнеар. Том 1.</t>
-        </is>
-      </c>
-      <c r="C429" t="n">
-        <v>520</v>
-      </c>
-      <c r="D429" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E429" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="430">
-      <c r="A430" s="1" t="n">
-        <v>428</v>
-      </c>
-      <c r="B430" t="inlineStr">
-        <is>
-          <t>Дровосечки. Побойся святого котенка. Том 1.</t>
-        </is>
-      </c>
-      <c r="C430" t="n">
-        <v>360</v>
-      </c>
-      <c r="D430" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E430" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="431">
-      <c r="A431" s="1" t="n">
-        <v>429</v>
-      </c>
-      <c r="B431" t="inlineStr">
-        <is>
-          <t>Округ Хэрроу. Том 1. Бесчисленные духи.</t>
-        </is>
-      </c>
-      <c r="C431" t="n">
-        <v>530</v>
-      </c>
-      <c r="D431" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E431" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="432">
-      <c r="A432" s="1" t="n">
-        <v>430</v>
-      </c>
-      <c r="B432" t="inlineStr">
-        <is>
-          <t>Арчи. Том 1.</t>
-        </is>
-      </c>
-      <c r="C432" t="n">
-        <v>395</v>
-      </c>
-      <c r="D432" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E432" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="433">
-      <c r="A433" s="1" t="n">
-        <v>431</v>
-      </c>
-      <c r="B433" t="inlineStr">
-        <is>
-          <t>Чудовище за соседней партой. Том 1.</t>
-        </is>
-      </c>
-      <c r="C433" t="n">
-        <v>355</v>
-      </c>
-      <c r="D433" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E433" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="434">
-      <c r="A434" s="1" t="n">
-        <v>432</v>
-      </c>
-      <c r="B434" t="inlineStr">
-        <is>
-          <t>Ангелы ковчега. Том 1.</t>
-        </is>
-      </c>
-      <c r="C434" t="n">
-        <v>280</v>
-      </c>
-      <c r="D434" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E434" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="435">
-      <c r="A435" s="1" t="n">
-        <v>433</v>
-      </c>
-      <c r="B435" t="inlineStr">
-        <is>
-          <t>Бездомный бог. Том 1.</t>
-        </is>
-      </c>
-      <c r="C435" t="n">
-        <v>355</v>
-      </c>
-      <c r="D435" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E435" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="436">
-      <c r="A436" s="1" t="n">
-        <v>434</v>
-      </c>
-      <c r="B436" t="inlineStr">
-        <is>
-          <t>Волчица и пряности. Том 13.</t>
-        </is>
-      </c>
-      <c r="C436" t="n">
-        <v>450</v>
-      </c>
-      <c r="D436" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E436" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="437">
-      <c r="A437" s="1" t="n">
-        <v>435</v>
-      </c>
-      <c r="B437" t="inlineStr">
-        <is>
-          <t>Волчица и пряности. Том 12.</t>
-        </is>
-      </c>
-      <c r="C437" t="n">
-        <v>450</v>
-      </c>
-      <c r="D437" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E437" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="438">
-      <c r="A438" s="1" t="n">
-        <v>436</v>
-      </c>
-      <c r="B438" t="inlineStr">
-        <is>
-          <t>В мире снов. Том 1</t>
-        </is>
-      </c>
-      <c r="C438" t="n">
-        <v>335</v>
-      </c>
-      <c r="D438" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E438" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="439">
-      <c r="A439" s="1" t="n">
-        <v>437</v>
-      </c>
-      <c r="B439" t="inlineStr">
-        <is>
-          <t>Деньги на бочку! Том 1.</t>
-        </is>
-      </c>
-      <c r="C439" t="n">
-        <v>245</v>
-      </c>
-      <c r="D439" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E439" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="440">
-      <c r="A440" s="1" t="n">
-        <v>438</v>
-      </c>
-      <c r="B440" t="inlineStr">
-        <is>
-          <t>Крушитель. Том 1.</t>
-        </is>
-      </c>
-      <c r="C440" t="n">
-        <v>320</v>
-      </c>
-      <c r="D440" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E440" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="441">
-      <c r="A441" s="1" t="n">
-        <v>439</v>
-      </c>
-      <c r="B441" t="inlineStr">
-        <is>
-          <t>Яростная месть. Том 1</t>
-        </is>
-      </c>
-      <c r="C441" t="n">
-        <v>335</v>
-      </c>
-      <c r="D441" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E441" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="442">
-      <c r="A442" s="1" t="n">
-        <v>440</v>
-      </c>
-      <c r="B442" t="inlineStr">
-        <is>
-          <t>Невеста чародея. Том 1</t>
-        </is>
-      </c>
-      <c r="C442" t="n">
-        <v>450</v>
-      </c>
-      <c r="D442" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E442" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="443">
-      <c r="A443" s="1" t="n">
-        <v>441</v>
-      </c>
-      <c r="B443" t="inlineStr">
-        <is>
-          <t>Бабочка. Том 1</t>
-        </is>
-      </c>
-      <c r="C443" t="n">
-        <v>335</v>
-      </c>
-      <c r="D443" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E443" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="444">
-      <c r="A444" s="1" t="n">
-        <v>442</v>
-      </c>
-      <c r="B444" t="inlineStr">
-        <is>
-          <t>Онинбо и адские личинки. Том 1</t>
-        </is>
-      </c>
-      <c r="C444" t="n">
-        <v>370</v>
-      </c>
-      <c r="D444" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E444" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="445">
-      <c r="A445" s="1" t="n">
-        <v>443</v>
-      </c>
-      <c r="B445" t="inlineStr">
-        <is>
-          <t>У меня мало друзей. Том 13.</t>
-        </is>
-      </c>
-      <c r="C445" t="n">
-        <v>260</v>
-      </c>
-      <c r="D445" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E445" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="446">
-      <c r="A446" s="1" t="n">
-        <v>444</v>
-      </c>
-      <c r="B446" t="inlineStr">
-        <is>
-          <t>У меня мало друзей. Том 1. Ver.1.1 (Исправленное и дополненное издание).</t>
-        </is>
-      </c>
-      <c r="C446" t="n">
-        <v>355</v>
-      </c>
-      <c r="D446" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E446" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="447">
-      <c r="A447" s="1" t="n">
-        <v>445</v>
-      </c>
-      <c r="B447" t="inlineStr">
-        <is>
-          <t>Изгой. Том 1.</t>
-        </is>
-      </c>
-      <c r="C447" t="n">
-        <v>530</v>
-      </c>
-      <c r="D447" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E447" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="448">
-      <c r="A448" s="1" t="n">
-        <v>446</v>
-      </c>
-      <c r="B448" t="inlineStr">
-        <is>
-          <t>Алиса в стране грехов. Принцип действия сна. Том 1.</t>
-        </is>
-      </c>
-      <c r="C448" t="n">
-        <v>370</v>
-      </c>
-      <c r="D448" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E448" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="449">
-      <c r="A449" s="1" t="n">
-        <v>447</v>
-      </c>
-      <c r="B449" t="inlineStr">
-        <is>
-          <t>Восхождение Героя Щита. Том 1.</t>
-        </is>
-      </c>
-      <c r="C449" t="n">
-        <v>355</v>
-      </c>
-      <c r="D449" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E449" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="450">
-      <c r="A450" s="1" t="n">
-        <v>448</v>
-      </c>
-      <c r="B450" t="inlineStr">
-        <is>
-          <t>All You Need Is Kill. Грань будущего. Том 1.</t>
-        </is>
-      </c>
-      <c r="C450" t="n">
-        <v>420</v>
-      </c>
-      <c r="D450" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E450" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="451">
-      <c r="A451" s="1" t="n">
-        <v>449</v>
-      </c>
-      <c r="B451" t="inlineStr">
-        <is>
-          <t>Рейдеры. Том 1.</t>
-        </is>
-      </c>
-      <c r="C451" t="n">
-        <v>255</v>
-      </c>
-      <c r="D451" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E451" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="452">
-      <c r="A452" s="1" t="n">
-        <v>450</v>
-      </c>
-      <c r="B452" t="inlineStr">
-        <is>
-          <t>Модель. Том 1</t>
-        </is>
-      </c>
-      <c r="C452" t="n">
-        <v>400</v>
-      </c>
-      <c r="D452" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E452" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="453">
-      <c r="A453" s="1" t="n">
-        <v>451</v>
-      </c>
-      <c r="B453" t="inlineStr">
-        <is>
-          <t>Redrum 327. Том 1</t>
-        </is>
-      </c>
-      <c r="C453" t="n">
-        <v>335</v>
-      </c>
-      <c r="D453" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E453" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="454">
-      <c r="A454" s="1" t="n">
-        <v>452</v>
-      </c>
-      <c r="B454" t="inlineStr">
-        <is>
-          <t>Небесный десант. Том 1</t>
-        </is>
-      </c>
-      <c r="C454" t="n">
-        <v>280</v>
-      </c>
-      <c r="D454" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E454" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="455">
-      <c r="A455" s="1" t="n">
-        <v>453</v>
-      </c>
-      <c r="B455" t="inlineStr">
-        <is>
-          <t>У меня мало друзей. Том 12.</t>
-        </is>
-      </c>
-      <c r="C455" t="n">
-        <v>260</v>
-      </c>
-      <c r="D455" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E455" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="456">
-      <c r="A456" s="1" t="n">
-        <v>454</v>
-      </c>
-      <c r="B456" t="inlineStr">
-        <is>
-          <t>Манга в Японии и России. Том 1.</t>
-        </is>
-      </c>
-      <c r="C456" t="n">
-        <v>610</v>
-      </c>
-      <c r="D456" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E456" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="457">
-      <c r="A457" s="1" t="n">
-        <v>455</v>
-      </c>
-      <c r="B457" t="inlineStr">
-        <is>
-          <t>Книга снов. Том 1.</t>
-        </is>
-      </c>
-      <c r="C457" t="n">
-        <v>280</v>
-      </c>
-      <c r="D457" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E457" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="458">
-      <c r="A458" s="1" t="n">
-        <v>456</v>
-      </c>
-      <c r="B458" t="inlineStr">
-        <is>
-          <t>Любовь онлайн. Том 1</t>
-        </is>
-      </c>
-      <c r="C458" t="n">
-        <v>280</v>
-      </c>
-      <c r="D458" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E458" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="459">
-      <c r="A459" s="1" t="n">
-        <v>457</v>
-      </c>
-      <c r="B459" t="inlineStr">
-        <is>
-          <t>Воспоминания маски. Том 1</t>
-        </is>
-      </c>
-      <c r="C459" t="n">
-        <v>370</v>
-      </c>
-      <c r="D459" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E459" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="460">
-      <c r="A460" s="1" t="n">
-        <v>458</v>
-      </c>
-      <c r="B460" t="inlineStr">
-        <is>
-          <t>Акира. Том 1.</t>
-        </is>
-      </c>
-      <c r="C460" t="n">
-        <v>975</v>
-      </c>
-      <c r="D460" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E460" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="461">
-      <c r="A461" s="1" t="n">
-        <v>459</v>
-      </c>
-      <c r="B461" t="inlineStr">
-        <is>
-          <t>Дюна. Графический роман. Том 1</t>
-        </is>
-      </c>
-      <c r="C461" t="n">
-        <v>930</v>
-      </c>
-      <c r="D461" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E461" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="462">
-      <c r="A462" s="1" t="n">
-        <v>460</v>
-      </c>
-      <c r="B462" t="inlineStr">
-        <is>
-          <t>Лунный Рыцарь. Том 1. Псих</t>
-        </is>
-      </c>
-      <c r="C462" t="n">
-        <v>445</v>
-      </c>
-      <c r="D462" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E462" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="463">
-      <c r="A463" s="1" t="n">
-        <v>461</v>
-      </c>
-      <c r="B463" t="inlineStr">
-        <is>
-          <t>Хвост Феи. Том 14.</t>
-        </is>
-      </c>
-      <c r="C463" t="n">
-        <v>365</v>
-      </c>
-      <c r="D463" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E463" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="464">
-      <c r="A464" s="1" t="n">
-        <v>462</v>
-      </c>
-      <c r="B464" t="inlineStr">
-        <is>
-          <t>Человек-Паук. Вызов. Том 1</t>
-        </is>
-      </c>
-      <c r="C464" t="n">
-        <v>1315</v>
-      </c>
-      <c r="D464" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E464" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="465">
-      <c r="A465" s="1" t="n">
-        <v>463</v>
-      </c>
-      <c r="B465" t="inlineStr">
-        <is>
-          <t>Хвост Феи. Том 13.</t>
-        </is>
-      </c>
-      <c r="C465" t="n">
-        <v>365</v>
-      </c>
-      <c r="D465" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E465" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="466">
-      <c r="A466" s="1" t="n">
-        <v>464</v>
-      </c>
-      <c r="B466" t="inlineStr">
-        <is>
-          <t>Проза бродячих псов. Том 1.</t>
-        </is>
-      </c>
-      <c r="C466" t="n">
-        <v>550</v>
-      </c>
-      <c r="D466" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E466" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="467">
-      <c r="A467" s="1" t="n">
-        <v>465</v>
-      </c>
-      <c r="B467" t="inlineStr">
-        <is>
-          <t>W.I.T.C.H. Чародейки. Часть 1. Двенадцать порталов. Том 1</t>
-        </is>
-      </c>
-      <c r="C467" t="n">
-        <v>900</v>
-      </c>
-      <c r="D467" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E467" t="inlineStr">
-        <is>
-          <t>Manga</t>
-        </is>
-      </c>
-    </row>
-    <row r="468">
-      <c r="A468" s="1" t="n">
-        <v>466</v>
-      </c>
-      <c r="B468" t="inlineStr">
-        <is>
-          <t>Ядерная зима. Том 1</t>
-        </is>
-      </c>
-      <c r="C468" t="n">
-        <v>450</v>
-      </c>
-      <c r="D468" t="inlineStr">
-        <is>
-          <t>XL Media</t>
-        </is>
-      </c>
-      <c r="E468" t="inlineStr">
         <is>
           <t>Manga</t>
         </is>

</xml_diff>

<commit_message>
1) Add "Nyaki" to shop list 2) Add Nyaki's goods to table
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E267"/>
+  <dimension ref="A1:E303"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1381,11 +1381,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Ранобэ Ты сияешь лунной ночью / Kimi wa Tsukiyo ni Hikari Kagayaku Том 1</t>
+          <t>Манга Магазинчик обуви / Shoe Store. Том 1</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>370</v>
+        <v>340</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1404,11 +1404,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Манга Магазинчик обуви / Shoe Store. Том 1</t>
+          <t>Манга Роскошный карат / Добродетель тьмы. Том 1</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1427,11 +1427,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Манга Роскошный карат / Добродетель тьмы. Том 1</t>
+          <t>Манга Интриги Ватсона и новый Шерлок Холмс / Watson no Inbou – Sherlock Holmes Ibun. Том 1</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>350</v>
+        <v>260</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -1450,11 +1450,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Манга Интриги Ватсона и новый Шерлок Холмс / Watson no Inbou – Sherlock Holmes Ibun. Том 1</t>
+          <t>Манга Неваляшка / Yajirobee. Том 1</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>260</v>
+        <v>400</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Манга Неваляшка / Yajirobee. Том 1</t>
+          <t>Манга Блаблабла / Kakukaku Shikajika. Том 1</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Манга Блаблабла / Kakukaku Shikajika. Том 1</t>
+          <t>Манга Дракорничная госпожи Кобаяси. Том 1</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1519,7 +1519,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Манга Дракорничная госпожи Кобаяси. Том 1</t>
+          <t>Манга Странные Дела. Том 1</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1542,11 +1542,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Манга Странные Дела. Том 1</t>
+          <t>Манга Илегенес. Симфония лжи / Ilegenes. Giyoku no Koukyoukyoku. Том 1</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>400</v>
+        <v>320</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1565,11 +1565,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Манга Илегенес. Симфония лжи / Ilegenes. Giyoku no Koukyoukyoku. Том 1</t>
+          <t>Манга Девушка у моря / Umibe no Onnanoko Том 1</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -1588,11 +1588,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Манга Девушка у моря / Umibe no Onnanoko Том 1</t>
+          <t>Манга Таймасин. Дневник экзорциста / Taimashin Том 1</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>340</v>
+        <v>370</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -1611,11 +1611,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Манга Таймасин. Дневник экзорциста / Taimashin Том 1</t>
+          <t>Манга Нелюдь / Ajin. Том 1</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>370</v>
+        <v>300</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -1634,11 +1634,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Манга Нелюдь / Ajin. Том 1</t>
+          <t>Манга Ну не может моя сестренка быть такой милой. Том 1</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -1657,11 +1657,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Манга Ну не может моя сестренка быть такой милой. Том 1</t>
+          <t>Манга Книга снов / Jade of Bango; Book of Dreams. Том 1</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>290</v>
+        <v>190</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1680,11 +1680,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Манга Книга снов / Jade of Bango; Book of Dreams. Том 1</t>
+          <t>Манга Железный миротворец / Peace Maker Kurogane. Том 1</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>190</v>
+        <v>260</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1703,11 +1703,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Манга Железный миротворец / Peace Maker Kurogane. Том 1</t>
+          <t>Манга Лунный мальчик / Moon Boy. Том 1</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1726,11 +1726,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Манга Лунный мальчик / Moon Boy. Том 1</t>
+          <t>Манга Номер один / The One. Том 1</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1749,11 +1749,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Манга Номер один / The One. Том 1</t>
+          <t>Манга Дневник демона / Demon Diary. Том 1</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>260</v>
+        <v>320</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1772,11 +1772,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Манга Дневник демона / Demon Diary. Том 1</t>
+          <t>Манга Староста-горничная! / The Student Council President is a Maid!  Том 1</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>320</v>
+        <v>240</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1795,11 +1795,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Манга Староста-горничная! / The Student Council President is a Maid!  Том 1</t>
+          <t>Манга Герой / Hero. Том 1</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -1818,11 +1818,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Манга Герой / Hero. Том 1</t>
+          <t>Манга Гостевой клуб лицея Оран / Ouran High School Host Club. Том 1</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -1841,11 +1841,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Манга Гостевой клуб лицея Оран / Ouran High School Host Club. Том 1</t>
+          <t>Манга Он и она и их обстоятельства / His and Her Circumstances. Том 1</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -1864,7 +1864,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Манга Он и она и их обстоятельства / His and Her Circumstances. Том 1</t>
+          <t>Манга Бабочка / Butterfly. Том 1</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1887,7 +1887,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Манга Бабочка / Butterfly. Том 1</t>
+          <t>Манга Джек Фрост / Jack Frost. Том 1</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1910,11 +1910,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Манга Джек Фрост / Jack Frost. Том 1</t>
+          <t>Манга Эмбрион мира / World Embryo. Том 1</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>260</v>
+        <v>420</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -1933,11 +1933,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Манга Эмбрион мира / World Embryo. Том 1</t>
+          <t>Манга Цветы зла / Evil Flowers. Том 1</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>420</v>
+        <v>280</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -1956,11 +1956,11 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Манга Цветы зла / Evil Flowers. Том 1</t>
+          <t>Манга Ночной изгнанник / Night Exile. Том 1</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -1979,7 +1979,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Манга Ночной изгнанник / Night Exile. Том 1</t>
+          <t>Манга Ателье “Paradise Kiss”. Том 1</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -2002,7 +2002,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Манга Ателье “Paradise Kiss”. Том 1</t>
+          <t>Манга Время героев / Heroes Lore. Wind of Soltia. Том 1</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -2025,11 +2025,11 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Манга Время героев / Heroes Lore. Wind of Soltia. Том 1</t>
+          <t>Манга Дикие клыки / Wild Fang. Том 1</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -2048,11 +2048,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Манга Дикие клыки / Wild Fang. Том 1</t>
+          <t>Манга Кантарелла / Cantarella. Том 1</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>250</v>
+        <v>190</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -2071,7 +2071,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Манга Кантарелла / Cantarella. Том 1</t>
+          <t>Манга Корона / Crown. Том 1</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -2094,11 +2094,11 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Манга Корона / Crown. Том 1</t>
+          <t>Манга Легенда о Лемнеар. Том 1</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>190</v>
+        <v>460</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -2117,11 +2117,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Манга Легенда о Лемнеар. Том 1</t>
+          <t>Манга Две стороны Мидзухо / Mizuho Ambivalent. Том 1</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>460</v>
+        <v>260</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -2140,11 +2140,11 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Манга Две стороны Мидзухо / Mizuho Ambivalent. Том 1</t>
+          <t>Манга Созвездие воображаемых зверей / Constellation of the Imaginary Beast. Том 1</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>260</v>
+        <v>310</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -2163,11 +2163,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Манга Созвездие воображаемых зверей / Constellation of the Imaginary Beast. Том 1</t>
+          <t>Манга Любовь Онлайн / Net Love. Том 1</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>310</v>
+        <v>260</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -2186,11 +2186,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Манга Любовь Онлайн / Net Love. Том 1</t>
+          <t>Манга Дисбаланс / Unbalance x Unbalance. Том 1</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -2209,11 +2209,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Манга Дисбаланс / Unbalance x Unbalance. Том 1</t>
+          <t>Манга Зеро. Нулевой образец / Zero. Том 1</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>270</v>
+        <v>320</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -2232,11 +2232,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Манга Зеро. Нулевой образец / Zero. Том 1</t>
+          <t>Манга Re:Play. Том 1</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>320</v>
+        <v>240</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -2255,11 +2255,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Манга Re:Play. Том 1</t>
+          <t>Манга Бланк / Blank. Том 1</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -2278,11 +2278,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Манга Бланк / Blank. Том 1</t>
+          <t>Манга Сладкий яд / Poison Candy. Том 1</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>260</v>
+        <v>130</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -2301,11 +2301,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Манга Сладкий яд / Poison Candy. Том 1</t>
+          <t>Манга Шоу уродов господина Араси / Dramacon. Том 1</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>130</v>
+        <v>420</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -2324,11 +2324,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Манга Шоу уродов господина Араси / Dramacon. Том 1</t>
+          <t>Манга Юная Королева Джун / Little Queen. Том 1</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>420</v>
+        <v>260</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -2347,11 +2347,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Манга Юная Королева Джун / Little Queen. Том 1</t>
+          <t>Манга Пустая шкатулка и нулевая Мария. Книга 1</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>260</v>
+        <v>550</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -2370,11 +2370,11 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Манга Пустая шкатулка и нулевая Мария. Книга 1</t>
+          <t>Манга Ария / Aria. Том 1</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>550</v>
+        <v>600</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -2393,11 +2393,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Манга Ария / Aria. Том 1</t>
+          <t>Манга Фиолетовое поле Лариона. Том 1</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>600</v>
+        <v>380</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -2416,11 +2416,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Манга Фиолетовое поле Лариона. Том 1</t>
+          <t>За гранью времен Г. Ф. Лавкрафта / H. P. Lovecraft’s Toki wo Koeru Kage. Том 1</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>380</v>
+        <v>350</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2439,11 +2439,11 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>За гранью времен Г. Ф. Лавкрафта / H. P. Lovecraft’s Toki wo Koeru Kage. Том 1</t>
+          <t>Манга Истории монстров. Том 1</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2462,11 +2462,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Манга Истории монстров. Том 1</t>
+          <t>Манга Знак Ватцеля / The Mark of Watzel. Том 1</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>330</v>
+        <v>400</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -2485,11 +2485,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Манга Знак Ватцеля / The Mark of Watzel. Том 1</t>
+          <t>Манга Ванильная глазурь / Vanilla Frosting. Том 1</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -2508,11 +2508,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Манга Ванильная глазурь / Vanilla Frosting. Том 1</t>
+          <t>Манга Дракон в поисках дома. Том 1</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -2531,11 +2531,11 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Манга Дракон в поисках дома. Том 1</t>
+          <t>Манга Манман-тян,ан! Священные узы. Том 1</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>400</v>
+        <v>260</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2554,7 +2554,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Манга Манман-тян,ан! Священные узы. Том 1</t>
+          <t>Манга Странная жизнь Субару / Subaru to Su-San. Том 1</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -2577,11 +2577,11 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Манга Странная жизнь Субару / Subaru to Su-San. Том 1</t>
+          <t>Манга Хребты безумия Г. Ф. Лавкрафта / H. P. Lovecraft’s At the Mountains of Madness. Том 1</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>260</v>
+        <v>350</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -2600,11 +2600,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Манга Хребты безумия Г. Ф. Лавкрафта / H. P. Lovecraft’s At the Mountains of Madness. Том 1</t>
+          <t>Манга Город, в котором меня нет / Boku dake ga Inai Machi. Том 1</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -2623,11 +2623,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Манга Город, в котором меня нет / Boku dake ga Inai Machi. Том 1</t>
+          <t>Манга Оружие мечты / GUNNM. Том 1</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -2646,11 +2646,11 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Манга Оружие мечты / GUNNM. Том 1</t>
+          <t>Манга Бандак / Bandak. Том 1</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>380</v>
+        <v>340</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -2669,11 +2669,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Манга Бандак / Bandak. Том 1</t>
+          <t>Манга Рыцари "Сидонии" / Sidonia no Kishi Том 1</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -2692,11 +2692,11 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Манга Рыцари "Сидонии" / Sidonia no Kishi Том 1</t>
+          <t>Манга Я - Сакамото, а что? / Sakamoto Desu ga? Том 1</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>320</v>
+        <v>280</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -2715,11 +2715,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Манга Я - Сакамото, а что? / Sakamoto Desu ga? Том 1</t>
+          <t>Манга Призрак в ночи / Ghost in the Dark. Том 1</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>280</v>
+        <v>400</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -2738,11 +2738,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Манга Призрак в ночи / Ghost in the Dark. Том 1</t>
+          <t>Манга Чудовище за соседней партой / Tonari no Kaibutsu-kun. Том 1</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>400</v>
+        <v>290</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -2761,11 +2761,11 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Манга Чудовище за соседней партой / Tonari no Kaibutsu-kun. Том 1</t>
+          <t>Манга Ангелы ковчега / Ark Angels. Том 1</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -2784,11 +2784,11 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Манга Ангелы ковчега / Ark Angels. Том 1</t>
+          <t>Манга Невеста чародея / Mahou Tsukai no Yome: Hoshi Matsu Hito. Том 1</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>260</v>
+        <v>400</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Манга Невеста чародея / Mahou Tsukai no Yome: Hoshi Matsu Hito. Том 1</t>
+          <t>Манга Оранж лайф. Том 1</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -2830,11 +2830,11 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Манга Оранж лайф. Том 1</t>
+          <t>Манга Священная мелодия. Нерассказанная история / Constellation of the Imaginary Beast. Том 1</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>400</v>
+        <v>260</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
@@ -2853,11 +2853,11 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Манга Священная мелодия. Нерассказанная история / Constellation of the Imaginary Beast. Том 1</t>
+          <t>Манга Хищная принцесса Егрина / Carnivorous Princess Yegrinna. Том 1</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>260</v>
+        <v>400</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -2876,11 +2876,11 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Манга Хищная принцесса Егрина / Carnivorous Princess Yegrinna. Том 1</t>
+          <t>Манга Опережая поцелуй / Faster than a kiss. Том 1</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>400</v>
+        <v>240</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
@@ -2899,11 +2899,11 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Манга Опережая поцелуй / Faster than a kiss. Том 1</t>
+          <t>Манга Оверман Король Гэйнер / Overman King Gainer. Том 1</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>240</v>
+        <v>190</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
@@ -2922,7 +2922,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Манга Оверман Король Гэйнер / Overman King Gainer. Том 1</t>
+          <t>Манга Двойная Спика / Twin Spica. Том 1</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -2945,11 +2945,11 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Манга Двойная Спика / Twin Spica. Том 1</t>
+          <t>Манга Призрачный мир / Ghost World. Том 1</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>190</v>
+        <v>250</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
@@ -2968,7 +2968,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Манга Призрачный мир / Ghost World. Том 1</t>
+          <t>Манга Гештальт / Gestalt. Том 1</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -2991,11 +2991,11 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Манга Гештальт / Gestalt. Том 1</t>
+          <t>Манга Сильнейший в истории ученик Кэнити / History's Strongest Disciple Kenichi. Том 1</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
@@ -3014,11 +3014,11 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Манга Сильнейший в истории ученик Кэнити / History's Strongest Disciple Kenichi. Том 1</t>
+          <t>Манга Легенда о Майане / The Legend of Maian. Том 1</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>260</v>
+        <v>200</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
@@ -3037,11 +3037,11 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Манга Легенда о Майане / The Legend of Maian. Том 1</t>
+          <t>Манга Принцесса-рыцарь. Том 1</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -3060,11 +3060,11 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Манга Принцесса-рыцарь. Том 1</t>
+          <t>Манга Рейдеры / Raiders. Том 1</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>280</v>
+        <v>240</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
@@ -3083,11 +3083,11 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Манга Рейдеры / Raiders. Том 1</t>
+          <t>Манга Творец фигурок / Figure Maker. Том 1</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>240</v>
+        <v>320</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
@@ -3106,7 +3106,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Манга Творец фигурок / Figure Maker. Том 1</t>
+          <t>Манга Охотник на ведьм / Witch Hunter. Том 1</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -3129,11 +3129,11 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Манга Охотник на ведьм / Witch Hunter. Том 1</t>
+          <t>Манга Излом / Shaman Warrior. Том 1</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>320</v>
+        <v>400</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
@@ -3152,7 +3152,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Манга Излом / Shaman Warrior. Том 1</t>
+          <t>Манга Скунс и оцелот. Том 1</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -3175,11 +3175,11 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Манга Скунс и оцелот. Том 1</t>
+          <t>Манга Подружки / Girl Friends. Том 1</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>400</v>
+        <v>280</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
@@ -3198,11 +3198,11 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Манга Подружки / Girl Friends. Том 1</t>
+          <t>Манга One. Том 1</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>280</v>
+        <v>230</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
@@ -3221,11 +3221,11 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Манга One. Том 1</t>
+          <t>Манга Школа лета  / Boys of Summer. Том 1</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>230</v>
+        <v>260</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
@@ -3244,11 +3244,11 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Манга Школа лета  / Boys of Summer. Том 1</t>
+          <t>Фигурка Юри на льду - Yuuri Katsuki</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>260</v>
+        <v>425</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
@@ -3257,7 +3257,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Figure</t>
         </is>
       </c>
     </row>
@@ -3267,11 +3267,11 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Фигурка Юри на льду - Yuuri Katsuki</t>
+          <t>Фигурка Fairy Tail: Canis Minor / Plue</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>425</v>
+        <v>170</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
@@ -3290,11 +3290,11 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Фигурка Fairy Tail: Canis Minor / Plue</t>
+          <t>Фигурка Pokemon - Snivy / Tsutarja</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>170</v>
+        <v>425</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
@@ -3313,7 +3313,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Фигурка Pokemon - Snivy / Tsutarja</t>
+          <t>Фигурка Юри на льду - Phichit Chulanont</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -3336,7 +3336,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Фигурка Юри на льду - Phichit Chulanont</t>
+          <t>Фигурка Юри на льду - Kenjirou Minami</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -3359,7 +3359,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Фигурка Юри на льду - Kenjirou Minami</t>
+          <t>Фигурка Sword Art Online SAO - Silica</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -3382,7 +3382,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Фигурка Sword Art Online SAO - Silica</t>
+          <t>Фигурка Sword Art Online SAO - Lisbeth</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -3405,7 +3405,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Фигурка Sword Art Online SAO - Lisbeth</t>
+          <t>Фигурка Sword Art Online SAO - Leafa</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -3428,11 +3428,11 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Фигурка Sword Art Online SAO - Leafa</t>
+          <t>Фигурка Card Captor Sakura №3</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>425</v>
+        <v>510</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
@@ -3451,11 +3451,11 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Фигурка Card Captor Sakura №3</t>
+          <t>Фигурка Touken Ranbu Online - Yamanbagiri Kunihiro</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>510</v>
+        <v>425</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
@@ -3474,7 +3474,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Фигурка Touken Ranbu Online - Yamanbagiri Kunihiro</t>
+          <t>Фигурка Kuroko no Basuke - Kise Ryota</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -3497,7 +3497,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke - Kise Ryota</t>
+          <t>Фигурка Kuroko no Basuke - Kagami Taiga</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -3520,7 +3520,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke - Kagami Taiga</t>
+          <t>Фигурка Kuroko no Basuke - Hyuga Junpei</t>
         </is>
       </c>
       <c r="C135" t="n">
@@ -3543,11 +3543,11 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke - Hyuga Junpei</t>
+          <t>Фигурка Vocaloid - Hatsune Miku  №6</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>425</v>
+        <v>680</v>
       </c>
       <c r="D136" t="inlineStr">
         <is>
@@ -3566,11 +3566,11 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Фигурка Vocaloid - Hatsune Miku  №6</t>
+          <t>Фигурка Kuroshitsuji: Lau</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>680</v>
+        <v>213</v>
       </c>
       <c r="D137" t="inlineStr">
         <is>
@@ -3589,11 +3589,11 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Фигурка Kuroshitsuji: Lau</t>
+          <t>Фигурка Kuroko no Basuke: Yukio Kasamatsu</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>213</v>
+        <v>425</v>
       </c>
       <c r="D138" t="inlineStr">
         <is>
@@ -3612,7 +3612,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Yukio Kasamatsu</t>
+          <t>Фигурка Kuroko no Basuke: Midorima Shintaro 310830</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -3635,7 +3635,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Midorima Shintaro 310830</t>
+          <t>Фигурка Kuroko no Basuke: Murasakibara Atsushi 310828</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -3658,7 +3658,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Murasakibara Atsushi 310828</t>
+          <t>Фигурка Kuroko no Basuke: Kagami Taiga 310827</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -3681,7 +3681,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Kagami Taiga 310827</t>
+          <t>Фигурка Kuroko no Basuke: Kuroko Tetsuya 310825</t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -3704,7 +3704,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Kuroko Tetsuya 310825</t>
+          <t>Фигурка Kuroko no Basuke: Murasakibara Atsushi 310822</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -3727,7 +3727,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Murasakibara Atsushi 310822</t>
+          <t>Фигурка Kuroko no Basuke: Kagami Taiga 310820</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -3750,11 +3750,11 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Kagami Taiga 310820</t>
+          <t>Фигурка Код Гиасс / Code Geass: Anya Alstreim</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>425</v>
+        <v>150</v>
       </c>
       <c r="D145" t="inlineStr">
         <is>
@@ -3773,11 +3773,11 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Фигурка Код Гиасс / Code Geass: Anya Alstreim</t>
+          <t>Фигурка Natsume Yuujinchou 70719</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>150</v>
+        <v>450</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
@@ -3796,11 +3796,11 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Фигурка Natsume Yuujinchou 70719</t>
+          <t>Фигурка Kuroshitsuji: Lau Tao 62415</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>450</v>
+        <v>170</v>
       </c>
       <c r="D147" t="inlineStr">
         <is>
@@ -3819,11 +3819,11 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Фигурка Kuroshitsuji: Lau Tao 62415</t>
+          <t>Фигурка Naruto: Konan 60787</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>170</v>
+        <v>340</v>
       </c>
       <c r="D148" t="inlineStr">
         <is>
@@ -3842,11 +3842,11 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Фигурка Naruto: Konan 60787</t>
+          <t>Фигурка Bleach - Abarai Renji</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>340</v>
+        <v>153</v>
       </c>
       <c r="D149" t="inlineStr">
         <is>
@@ -3865,11 +3865,11 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Фигурка Bleach - Abarai Renji</t>
+          <t>Фигурка Kuroshitsuji: Madam Red</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>153</v>
+        <v>425</v>
       </c>
       <c r="D150" t="inlineStr">
         <is>
@@ -3888,11 +3888,11 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Фигурка Kuroshitsuji: Madam Red</t>
+          <t>Фигурка Inu Yasha 31344</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>425</v>
+        <v>255</v>
       </c>
       <c r="D151" t="inlineStr">
         <is>
@@ -3911,11 +3911,11 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Фигурка Inu Yasha 31344</t>
+          <t>Фигурка Ranma 1/2 31342</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D152" t="inlineStr">
         <is>
@@ -3934,7 +3934,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Фигурка Ranma 1/2 31342</t>
+          <t>Фигурка Ranma 1/2  31338</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -3957,11 +3957,11 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Фигурка Ranma 1/2  31338</t>
+          <t>Копия фигурки Tokyo Ghoul FG31063-4</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>250</v>
+        <v>1190</v>
       </c>
       <c r="D154" t="inlineStr">
         <is>
@@ -3980,11 +3980,11 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Копия фигурки Tokyo Ghoul FG31063-4</t>
+          <t>Копия фигурки Natsume Yuujinchou PVC Figure NYFR04</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>1190</v>
+        <v>680</v>
       </c>
       <c r="D155" t="inlineStr">
         <is>
@@ -4003,11 +4003,11 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Копия фигурки Natsume Yuujinchou PVC Figure NYFR04</t>
+          <t>Фигурка Kuroko no Basuke: Takao Kazunari 510442</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>680</v>
+        <v>425</v>
       </c>
       <c r="D156" t="inlineStr">
         <is>
@@ -4026,11 +4026,11 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Набор фигурок My Neighbor Totoro PVC Figures Set TOFR02</t>
+          <t>Фигурка Kuroko no Basuke: Daiki Aomine</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>1700</v>
+        <v>425</v>
       </c>
       <c r="D157" t="inlineStr">
         <is>
@@ -4049,11 +4049,11 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Набор фигурок My Neighbor Totoro PVC Figures Set TOFR01</t>
+          <t>Фигурка Love Live! Sunshine!! - Koidzumi Hanayo</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>1700</v>
+        <v>765</v>
       </c>
       <c r="D158" t="inlineStr">
         <is>
@@ -4072,11 +4072,11 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Takao Kazunari 510442</t>
+          <t>Фигурка Card Captor Sakura №5</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>425</v>
+        <v>510</v>
       </c>
       <c r="D159" t="inlineStr">
         <is>
@@ -4095,11 +4095,11 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Daiki Aomine</t>
+          <t>Фигурка Fate Extella -  Archimedes</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>425</v>
+        <v>510</v>
       </c>
       <c r="D160" t="inlineStr">
         <is>
@@ -4118,11 +4118,11 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Фигурка Love Live! Sunshine!! - Koidzumi Hanayo</t>
+          <t>Фигурка Fate Extella - Attila</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>765</v>
+        <v>510</v>
       </c>
       <c r="D161" t="inlineStr">
         <is>
@@ -4141,11 +4141,11 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Фигурка Card Captor Sakura №5</t>
+          <t>Фигурка Touken Ranbu Online - Hirano Toushirou</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>510</v>
+        <v>425</v>
       </c>
       <c r="D162" t="inlineStr">
         <is>
@@ -4164,11 +4164,11 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Фигурка Fate Extella -  Archimedes</t>
+          <t>Фигурка Touken Ranbu Online - Souza Samonji</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>510</v>
+        <v>425</v>
       </c>
       <c r="D163" t="inlineStr">
         <is>
@@ -4187,11 +4187,11 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Фигурка Fate Extella - Attila</t>
+          <t>Фигурка Touken Ranbu Online -Kikkou Sadamune</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>510</v>
+        <v>425</v>
       </c>
       <c r="D164" t="inlineStr">
         <is>
@@ -4210,7 +4210,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Фигурка Touken Ranbu Online - Hirano Toushirou</t>
+          <t>Фигурка Touken Ranbu Online - Yagen Toushirou</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -4233,11 +4233,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Фигурка Touken Ranbu Online - Souza Samonji</t>
+          <t>Фигурка Баскетбол Куроко - Казунари Такао</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>425</v>
+        <v>510</v>
       </c>
       <c r="D166" t="inlineStr">
         <is>
@@ -4256,11 +4256,11 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Фигурка Touken Ranbu Online -Kikkou Sadamune</t>
+          <t>Фигурка Баскетбол Куроко - Шоичи Имаёши</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>425</v>
+        <v>510</v>
       </c>
       <c r="D167" t="inlineStr">
         <is>
@@ -4279,7 +4279,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Фигурка Touken Ranbu Online - Yagen Toushirou</t>
+          <t>Фигурка Kuroko no Basuke - Takao Kazunari</t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -4302,11 +4302,11 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Фигурка Баскетбол Куроко - Казунари Такао</t>
+          <t>Фигурка Vocaloid - Hatsune Miku  №5</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>510</v>
+        <v>680</v>
       </c>
       <c r="D169" t="inlineStr">
         <is>
@@ -4325,11 +4325,11 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Фигурка Баскетбол Куроко - Шоичи Имаёши</t>
+          <t>Фигурка Vocaloid - Hatsune Miku №4</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>510</v>
+        <v>680</v>
       </c>
       <c r="D170" t="inlineStr">
         <is>
@@ -4348,11 +4348,11 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke - Takao Kazunari</t>
+          <t>Набор фигурок Kantai Collection (9 штук)</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>425</v>
+        <v>3740</v>
       </c>
       <c r="D171" t="inlineStr">
         <is>
@@ -4371,11 +4371,11 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Фигурка Vocaloid - Hatsune Miku  №5</t>
+          <t>Фигурка Kuroko no Basuke: Kensuke Fukui</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>680</v>
+        <v>213</v>
       </c>
       <c r="D172" t="inlineStr">
         <is>
@@ -4394,11 +4394,11 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Фигурка Vocaloid - Hatsune Miku №4</t>
+          <t>Фигурка Kuroko no Basuke: Akashi Seijuro 315637</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>680</v>
+        <v>425</v>
       </c>
       <c r="D173" t="inlineStr">
         <is>
@@ -4417,11 +4417,11 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Набор фигурок Kantai Collection (9 штук)</t>
+          <t>Фигурка Kuroko no Basuke: Takao Kazunari 315636</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>3740</v>
+        <v>425</v>
       </c>
       <c r="D174" t="inlineStr">
         <is>
@@ -4440,11 +4440,11 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Фигурка Katekyo Hitman Reborn! - Ryouhei Sasagawa</t>
+          <t>Фигурка Kuroko no Basuke: Hanamiya Makoto</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>340</v>
+        <v>425</v>
       </c>
       <c r="D175" t="inlineStr">
         <is>
@@ -4463,11 +4463,11 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Копия фигурки Gintama Sogo Okita</t>
+          <t>Фигурка Kuroko no Basuke: Himuro Tatsuya 315634</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>680</v>
+        <v>425</v>
       </c>
       <c r="D176" t="inlineStr">
         <is>
@@ -4486,11 +4486,11 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Kensuke Fukui</t>
+          <t>Фигурка Kuroko no Basuke: Aomine Daiki</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>213</v>
+        <v>425</v>
       </c>
       <c r="D177" t="inlineStr">
         <is>
@@ -4509,7 +4509,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Akashi Seijuro 315637</t>
+          <t>Фигурка Kuroko no Basuke: Kise Ryota 310826</t>
         </is>
       </c>
       <c r="C178" t="n">
@@ -4532,7 +4532,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Takao Kazunari 315636</t>
+          <t>Фигурка Kuroko no Basuke: Kasamatsu Yukio</t>
         </is>
       </c>
       <c r="C179" t="n">
@@ -4555,7 +4555,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Hanamiya Makoto</t>
+          <t>Фигурка Kuroko no Basuke: Kuroko Tetsuya 310823</t>
         </is>
       </c>
       <c r="C180" t="n">
@@ -4578,7 +4578,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Himuro Tatsuya 315634</t>
+          <t>Фигурка Kuroko no Basuke: Himuro Tatsuya 310821</t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -4601,11 +4601,11 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Aomine Daiki</t>
+          <t>Фигурка Rurouni Kenshin: Shinomori Aoshi</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>425</v>
+        <v>221</v>
       </c>
       <c r="D182" t="inlineStr">
         <is>
@@ -4624,15 +4624,15 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Kise Ryota 310826</t>
+          <t>Nendoroid Nikki</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>425</v>
+        <v>4553</v>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>XL Media</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
@@ -4647,15 +4647,15 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Kasamatsu Yukio</t>
+          <t>Nendoroid Amaterasu DX Ver.</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>425</v>
+        <v>8967</v>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>XL Media</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
@@ -4670,15 +4670,15 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Kuroko Tetsuya 310823</t>
+          <t>Nendoroid Hunter: Male Zinogre Alpha Armor Ver. DX</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>425</v>
+        <v>6295</v>
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>XL Media</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
@@ -4693,15 +4693,15 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Фигурка Kuroko no Basuke: Himuro Tatsuya 310821</t>
+          <t>Nendoroid Shizue (Isabelle): Winter Ver.</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>425</v>
+        <v>5722</v>
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>XL Media</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
@@ -4716,15 +4716,15 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Фигурка Rurouni Kenshin: Shinomori Aoshi</t>
+          <t>Nendoroid Orphen</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>221</v>
+        <v>4175</v>
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>XL Media</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
@@ -4739,15 +4739,15 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Набор фигурок DRAMAtical Murder</t>
+          <t>Nendoroid Tenya Iida</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>2992</v>
+        <v>4594</v>
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>XL Media</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
@@ -4762,15 +4762,15 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Набор фигурок Shingeki no Kyojin / Attack on Titan: Annie Leonheart +1</t>
+          <t>Nendoroid Ena Saito</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>1309</v>
+        <v>7495</v>
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>XL Media</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
@@ -4785,15 +4785,15 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Фигурка аниме 83498</t>
+          <t>Nendoroid Rin Shima: Touring Ver.</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>187</v>
+        <v>6565</v>
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>XL Media</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
@@ -4808,15 +4808,15 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Фигурка аниме 83497</t>
+          <t>Nendoroid Sakura Amamiya</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>149</v>
+        <v>4043</v>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>XL Media</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
@@ -4831,15 +4831,15 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Копия фигурки Vocaloid: Hatsune Miku 83000</t>
+          <t>Nendoroid Avenger/Jeanne d'Arc (Alter) Shinjuku Ver.</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>340</v>
+        <v>5892</v>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>XL Media</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
@@ -4854,15 +4854,15 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Фигурка Code Geass: Anya Alstreim</t>
+          <t>Nendoroid Archer/Gilgamesh: Third Ascension Ver.</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>170</v>
+        <v>5679</v>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>XL Media</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
@@ -4877,15 +4877,15 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Фигурка Code Geass: Gino Weinberg 70785</t>
+          <t>Nendoroid Hatsune Miku V4X</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>170</v>
+        <v>6426</v>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>XL Media</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
@@ -4900,15 +4900,15 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Фигурка Code Geass: Gino Weinberg 70784</t>
+          <t>Nendoroid Shinichi Kudo</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>85</v>
+        <v>4161</v>
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>XL Media</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
@@ -4923,15 +4923,15 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Фигурка Gintama: Kintoki Sakata 70087</t>
+          <t>Nendoroid Doll Hatsune Miku</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>374</v>
+        <v>7955</v>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>XL Media</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
@@ -4946,20 +4946,20 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Фигурка Chobits 61963</t>
+          <t>Проза бродячих псов. Том 1.</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>94</v>
+        <v>550</v>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>XL Media</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>Figure</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -4969,11 +4969,11 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Nendoroid Nikki</t>
+          <t>Акира. Том 1.</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>4553</v>
+        <v>975</v>
       </c>
       <c r="D198" t="inlineStr">
         <is>
@@ -4982,7 +4982,7 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>Figure</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -4992,11 +4992,11 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Nendoroid Amaterasu DX Ver.</t>
+          <t>Семь смертных грехов. Том 1.</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>8967</v>
+        <v>550</v>
       </c>
       <c r="D199" t="inlineStr">
         <is>
@@ -5005,7 +5005,7 @@
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>Figure</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -5015,11 +5015,11 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Nendoroid Hunter: Male Zinogre Alpha Armor Ver. DX</t>
+          <t>Истории монстров. Том 1.</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>6295</v>
+        <v>355</v>
       </c>
       <c r="D200" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>Figure</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -5038,11 +5038,11 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Nendoroid Shizue (Isabelle): Winter Ver.</t>
+          <t>Тетрадь дружбы Нацумэ. Том 1.</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>5722</v>
+        <v>550</v>
       </c>
       <c r="D201" t="inlineStr">
         <is>
@@ -5051,7 +5051,7 @@
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>Figure</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -5061,11 +5061,11 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Nendoroid Orphen</t>
+          <t>Sailor Moon. Том 1.</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>4175</v>
+        <v>390</v>
       </c>
       <c r="D202" t="inlineStr">
         <is>
@@ -5074,7 +5074,7 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>Figure</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -5084,11 +5084,11 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Nendoroid Tenya Iida</t>
+          <t>Бездомный бог. Том 1.</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4594</v>
+        <v>355</v>
       </c>
       <c r="D203" t="inlineStr">
         <is>
@@ -5097,7 +5097,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>Figure</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -5107,11 +5107,11 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Nendoroid Ena Saito</t>
+          <t>Ты сияешь лунной ночью. Том 1.</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>7495</v>
+        <v>355</v>
       </c>
       <c r="D204" t="inlineStr">
         <is>
@@ -5120,7 +5120,7 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>Figure</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -5130,11 +5130,11 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Nendoroid Rin Shima: Touring Ver.</t>
+          <t>Восхождение Героя Щита. Том 1.</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>6565</v>
+        <v>355</v>
       </c>
       <c r="D205" t="inlineStr">
         <is>
@@ -5143,7 +5143,7 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>Figure</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -5153,11 +5153,11 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Nendoroid Sakura Amamiya</t>
+          <t>Врата;Штейна 0. Том 1.</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>4043</v>
+        <v>355</v>
       </c>
       <c r="D206" t="inlineStr">
         <is>
@@ -5166,7 +5166,7 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>Figure</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -5176,11 +5176,11 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Nendoroid Avenger/Jeanne d'Arc (Alter) Shinjuku Ver.</t>
+          <t>Созданный в Бездне. Том 1</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>5892</v>
+        <v>360</v>
       </c>
       <c r="D207" t="inlineStr">
         <is>
@@ -5189,7 +5189,7 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>Figure</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -5199,11 +5199,11 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Nendoroid Archer/Gilgamesh: Third Ascension Ver.</t>
+          <t>Хвост Феи. Том 10.</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>5679</v>
+        <v>365</v>
       </c>
       <c r="D208" t="inlineStr">
         <is>
@@ -5212,7 +5212,7 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>Figure</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -5222,11 +5222,11 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Nendoroid Hatsune Miku V4X</t>
+          <t>Без игры жизни нет. Том 1.</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>6426</v>
+        <v>355</v>
       </c>
       <c r="D209" t="inlineStr">
         <is>
@@ -5235,7 +5235,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>Figure</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -5245,11 +5245,11 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Nendoroid Shinichi Kudo</t>
+          <t>Ложные выводы. Том 1</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>4161</v>
+        <v>530</v>
       </c>
       <c r="D210" t="inlineStr">
         <is>
@@ -5258,7 +5258,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>Figure</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -5268,11 +5268,11 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Nendoroid Doll Hatsune Miku</t>
+          <t>«Страна чудес смертников». Том 1</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>7955</v>
+        <v>355</v>
       </c>
       <c r="D211" t="inlineStr">
         <is>
@@ -5281,7 +5281,7 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>Figure</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -5291,11 +5291,11 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Проза бродячих псов. Том 1.</t>
+          <t>У меня мало друзей. Том 1. Ver.1.1 (Исправленное и дополненное издание).</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>550</v>
+        <v>355</v>
       </c>
       <c r="D212" t="inlineStr">
         <is>
@@ -5314,11 +5314,11 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Акира. Том 1.</t>
+          <t>Хвост Феи. Том 1.</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>975</v>
+        <v>365</v>
       </c>
       <c r="D213" t="inlineStr">
         <is>
@@ -5337,11 +5337,11 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Семь смертных грехов. Том 1.</t>
+          <t>Торадора! Том 1.</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>550</v>
+        <v>255</v>
       </c>
       <c r="D214" t="inlineStr">
         <is>
@@ -5360,11 +5360,11 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Истории монстров. Том 1.</t>
+          <t>Необъятный океан. Том 1.</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>355</v>
+        <v>530</v>
       </c>
       <c r="D215" t="inlineStr">
         <is>
@@ -5383,11 +5383,11 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Тетрадь дружбы Нацумэ. Том 1.</t>
+          <t>Врата;Штейна. Том 1</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>550</v>
+        <v>355</v>
       </c>
       <c r="D216" t="inlineStr">
         <is>
@@ -5406,11 +5406,11 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Sailor Moon. Том 1.</t>
+          <t>Последнее путешествие девочек. Том 1</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>390</v>
+        <v>510</v>
       </c>
       <c r="D217" t="inlineStr">
         <is>
@@ -5429,11 +5429,11 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Бездомный бог. Том 1.</t>
+          <t>Научное доказательство любви. Том 1.</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="D218" t="inlineStr">
         <is>
@@ -5452,11 +5452,11 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Ты сияешь лунной ночью. Том 1.</t>
+          <t>GUNNM. Том 1.</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="D219" t="inlineStr">
         <is>
@@ -5475,11 +5475,11 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Восхождение Героя Щита. Том 1.</t>
+          <t>Blame! Том 1.</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="D220" t="inlineStr">
         <is>
@@ -5498,11 +5498,11 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Врата;Штейна 0. Том 1.</t>
+          <t>Эльф не может похудеть. Том 1</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="D221" t="inlineStr">
         <is>
@@ -5521,11 +5521,11 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Созданный в Бездне. Том 1</t>
+          <t>Паразит. Том 1.</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>360</v>
+        <v>495</v>
       </c>
       <c r="D222" t="inlineStr">
         <is>
@@ -5544,11 +5544,11 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Хвост Феи. Том 10.</t>
+          <t>Я - Сакамото, а что? Том 1.</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="D223" t="inlineStr">
         <is>
@@ -5567,11 +5567,11 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Без игры жизни нет. Том 1.</t>
+          <t>Ария. Том 1.</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>355</v>
+        <v>645</v>
       </c>
       <c r="D224" t="inlineStr">
         <is>
@@ -5590,11 +5590,11 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Ложные выводы. Том 1</t>
+          <t>Город кислоты. Том 1. Ver.1.1 (Исправленное и дополненное издание).</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>530</v>
+        <v>355</v>
       </c>
       <c r="D225" t="inlineStr">
         <is>
@@ -5613,11 +5613,11 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>«Страна чудес смертников». Том 1</t>
+          <t>Бдительный Эгути-кун. Том 1</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>355</v>
+        <v>275</v>
       </c>
       <c r="D226" t="inlineStr">
         <is>
@@ -5636,11 +5636,11 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>У меня мало друзей. Том 1. Ver.1.1 (Исправленное и дополненное издание).</t>
+          <t>Скитания Эманон. Том 1.</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>355</v>
+        <v>390</v>
       </c>
       <c r="D227" t="inlineStr">
         <is>
@@ -5659,11 +5659,11 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Хвост Феи. Том 1.</t>
+          <t>Нелюдь. Том 1.</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="D228" t="inlineStr">
         <is>
@@ -5682,11 +5682,11 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Торадора! Том 1.</t>
+          <t>Чудовище за соседней партой. Том 1.</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>255</v>
+        <v>355</v>
       </c>
       <c r="D229" t="inlineStr">
         <is>
@@ -5705,11 +5705,11 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Необъятный океан. Том 1.</t>
+          <t>Рыцари «Сидонии». Том 1.</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>530</v>
+        <v>300</v>
       </c>
       <c r="D230" t="inlineStr">
         <is>
@@ -5728,7 +5728,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Врата;Штейна. Том 1</t>
+          <t>Загадка Дьявола. Том 1.</t>
         </is>
       </c>
       <c r="C231" t="n">
@@ -5751,11 +5751,11 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Последнее путешествие девочек. Том 1</t>
+          <t>Тетрадь Смерти: Black Edition. Книга 1</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>510</v>
+        <v>805</v>
       </c>
       <c r="D232" t="inlineStr">
         <is>
@@ -5774,11 +5774,11 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Научное доказательство любви. Том 1.</t>
+          <t>Нахальный принц и кошка-несмеяна. Том 1. Ver.1.1 (Исправленное и дополненное издание).</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D233" t="inlineStr">
         <is>
@@ -5797,11 +5797,11 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>GUNNM. Том 1.</t>
+          <t>All You Need Is Kill. Грань будущего. Том 1.</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>375</v>
+        <v>420</v>
       </c>
       <c r="D234" t="inlineStr">
         <is>
@@ -5820,11 +5820,11 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Blame! Том 1.</t>
+          <t>Странники. Том 1.</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>315</v>
+        <v>470</v>
       </c>
       <c r="D235" t="inlineStr">
         <is>
@@ -5843,11 +5843,11 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Эльф не может похудеть. Том 1</t>
+          <t>Аква. Том 1.</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>340</v>
+        <v>280</v>
       </c>
       <c r="D236" t="inlineStr">
         <is>
@@ -5866,11 +5866,11 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Паразит. Том 1.</t>
+          <t>Бакуман. Книга 1</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>495</v>
+        <v>539</v>
       </c>
       <c r="D237" t="inlineStr">
         <is>
@@ -5889,11 +5889,11 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Я - Сакамото, а что? Том 1.</t>
+          <t>Дабл ми. Том 1.</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="D238" t="inlineStr">
         <is>
@@ -5912,11 +5912,11 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Ария. Том 1.</t>
+          <t>Милый дом Чи. Книга 1</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>645</v>
+        <v>305</v>
       </c>
       <c r="D239" t="inlineStr">
         <is>
@@ -5935,20 +5935,20 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Город кислоты. Том 1. Ver.1.1 (Исправленное и дополненное издание).</t>
+          <t>Набор значков Haikyuu!!</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>355</v>
+        <v>500</v>
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>XL Media</t>
+          <t>Discomir</t>
         </is>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Pins</t>
         </is>
       </c>
     </row>
@@ -5958,20 +5958,20 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Бдительный Эгути-кун. Том 1</t>
+          <t>Набор больших значков "Haikyuu!!"</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>275</v>
+        <v>300</v>
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>XL Media</t>
+          <t>Discomir</t>
         </is>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Pins</t>
         </is>
       </c>
     </row>
@@ -5981,20 +5981,20 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Скитания Эманон. Том 1.</t>
+          <t>Набор значков Haikyuu!!</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>390</v>
+        <v>500</v>
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>XL Media</t>
+          <t>Discomir</t>
         </is>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Pins</t>
         </is>
       </c>
     </row>
@@ -6004,20 +6004,20 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Нелюдь. Том 1.</t>
+          <t>Набор больших значков "Haikyuu!!"</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>355</v>
+        <v>300</v>
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>XL Media</t>
+          <t>Discomir</t>
         </is>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Pins</t>
         </is>
       </c>
     </row>
@@ -6027,20 +6027,20 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Чудовище за соседней партой. Том 1.</t>
+          <t>Набор больших значков "Haikyuu!!"</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>355</v>
+        <v>300</v>
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>XL Media</t>
+          <t>Discomir</t>
         </is>
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Pins</t>
         </is>
       </c>
     </row>
@@ -6050,7 +6050,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Рыцари «Сидонии». Том 1.</t>
+          <t>Набор больших значков "Banana Fish"</t>
         </is>
       </c>
       <c r="C245" t="n">
@@ -6058,12 +6058,12 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>XL Media</t>
+          <t>Discomir</t>
         </is>
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Pins</t>
         </is>
       </c>
     </row>
@@ -6073,20 +6073,20 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Загадка Дьявола. Том 1.</t>
+          <t>Набор больших значков "Haikyuu!!"</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>355</v>
+        <v>300</v>
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>XL Media</t>
+          <t>Discomir</t>
         </is>
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Pins</t>
         </is>
       </c>
     </row>
@@ -6096,20 +6096,20 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Тетрадь Смерти: Black Edition. Книга 1</t>
+          <t>Набор значков Kobayashi-san Chi no Maid Dragon</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>805</v>
+        <v>500</v>
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>XL Media</t>
+          <t>Discomir</t>
         </is>
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Pins</t>
         </is>
       </c>
     </row>
@@ -6119,20 +6119,20 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Нахальный принц и кошка-несмеяна. Том 1. Ver.1.1 (Исправленное и дополненное издание).</t>
+          <t>Набор больших значков "Kobayashi-san Chi no Maid Dragon"</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>355</v>
+        <v>300</v>
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>XL Media</t>
+          <t>Discomir</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Pins</t>
         </is>
       </c>
     </row>
@@ -6142,20 +6142,20 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>All You Need Is Kill. Грань будущего. Том 1.</t>
+          <t>Набор больших значков "Dr. Stone"</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>420</v>
+        <v>300</v>
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>XL Media</t>
+          <t>Discomir</t>
         </is>
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Pins</t>
         </is>
       </c>
     </row>
@@ -6165,20 +6165,20 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Странники. Том 1.</t>
+          <t>Набор больших значков "Dr. Stone"</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>470</v>
+        <v>300</v>
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>XL Media</t>
+          <t>Discomir</t>
         </is>
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Pins</t>
         </is>
       </c>
     </row>
@@ -6188,20 +6188,20 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Аква. Том 1.</t>
+          <t>Набор значков "Dr. Stone"</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>280</v>
+        <v>500</v>
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>XL Media</t>
+          <t>Discomir</t>
         </is>
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Pins</t>
         </is>
       </c>
     </row>
@@ -6211,20 +6211,20 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Бакуман. Книга 1</t>
+          <t>Набор больших значков "Aho Girl"</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>539</v>
+        <v>300</v>
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>XL Media</t>
+          <t>Discomir</t>
         </is>
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>Manga</t>
+          <t>Pins</t>
         </is>
       </c>
     </row>
@@ -6234,15 +6234,15 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Дабл ми. Том 1.</t>
+          <t>Манга "Наруто", 1 книга</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>335</v>
+        <v>690</v>
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>XL Media</t>
+          <t>Nyaki</t>
         </is>
       </c>
       <c r="E253" t="inlineStr">
@@ -6257,15 +6257,15 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Милый дом Чи. Книга 1</t>
+          <t>Манга "Обещанная страна грёз", 1 том</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>305</v>
+        <v>750</v>
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>XL Media</t>
+          <t>Nyaki</t>
         </is>
       </c>
       <c r="E254" t="inlineStr">
@@ -6280,20 +6280,20 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Набор значков Haikyuu!!</t>
+          <t>Манга "Моя геройская академия", 1 книга</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>Nyaki</t>
         </is>
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>Pins</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -6303,20 +6303,20 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Набор больших значков "Haikyuu!!"</t>
+          <t>Манга "Стальной Алхимик", 1 книга</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>300</v>
+        <v>750</v>
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>Nyaki</t>
         </is>
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>Pins</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -6326,20 +6326,20 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Набор значков Haikyuu!!</t>
+          <t>Манга "Без игры жизни нет", 1 том</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>500</v>
+        <v>390</v>
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>Nyaki</t>
         </is>
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>Pins</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -6349,20 +6349,20 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Набор больших значков "Haikyuu!!"</t>
+          <t>Манга "Призрак в доспехах", 1 том</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>300</v>
+        <v>890</v>
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>Nyaki</t>
         </is>
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>Pins</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -6372,20 +6372,20 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Набор больших значков "Haikyuu!!"</t>
+          <t>Манга "Научное доказательство любви", 1 том</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>300</v>
+        <v>390</v>
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>Nyaki</t>
         </is>
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>Pins</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -6395,20 +6395,20 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Набор больших значков "Banana Fish"</t>
+          <t>Манга "Я - Сакамото, а что?", 1 том</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>300</v>
+        <v>390</v>
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>Nyaki</t>
         </is>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>Pins</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -6418,20 +6418,20 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Набор больших значков "Haikyuu!!"</t>
+          <t>Манга "Необъятный океан", 1 том</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>300</v>
+        <v>490</v>
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>Nyaki</t>
         </is>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>Pins</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -6441,20 +6441,20 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Набор значков Kobayashi-san Chi no Maid Dragon</t>
+          <t>Манга "Твоя апрельская ложь", 1 том</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>500</v>
+        <v>390</v>
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>Nyaki</t>
         </is>
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>Pins</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -6464,20 +6464,20 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Набор больших значков "Kobayashi-san Chi no Maid Dragon"</t>
+          <t>Манга "Сага о Винланде", 1 книга</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>300</v>
+        <v>750</v>
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>Nyaki</t>
         </is>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>Pins</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -6487,20 +6487,20 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Набор больших значков "Dr. Stone"</t>
+          <t>Манга "Сердца Пандоры", 1 книга</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>300</v>
+        <v>650</v>
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>Nyaki</t>
         </is>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Pins</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -6510,20 +6510,20 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Набор больших значков "Dr. Stone"</t>
+          <t>Манга "Токийский гуль: re", 1 книга</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>300</v>
+        <v>590</v>
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>Nyaki</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>Pins</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -6533,20 +6533,20 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Набор значков "Dr. Stone"</t>
+          <t>Манга "Восхождение Героя Щита", 1 том</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>500</v>
+        <v>380</v>
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Discomir</t>
+          <t>Nyaki</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>Pins</t>
+          <t>Manga</t>
         </is>
       </c>
     </row>
@@ -6556,20 +6556,848 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Набор больших значков "Aho Girl"</t>
+          <t>Манга "Re:Zero. Жизнь с нуля в альтернативном мире. День в столице королевства", 1 том</t>
         </is>
       </c>
       <c r="C267" t="n">
+        <v>390</v>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="1" t="n">
+        <v>266</v>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>Манга "Тетрадь дружбы Нацумэ", 1 том</t>
+        </is>
+      </c>
+      <c r="C268" t="n">
+        <v>590</v>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Манга "Врата штейна", 1 том</t>
+        </is>
+      </c>
+      <c r="C269" t="n">
+        <v>390</v>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="1" t="n">
+        <v>268</v>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>Манга "Нелюдь", 1 том</t>
+        </is>
+      </c>
+      <c r="C270" t="n">
+        <v>390</v>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="1" t="n">
+        <v>269</v>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>Манга "Истории монстров", 1 том</t>
+        </is>
+      </c>
+      <c r="C271" t="n">
+        <v>380</v>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="1" t="n">
+        <v>270</v>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>Манга "Так сложно любить отаку", 1 том</t>
+        </is>
+      </c>
+      <c r="C272" t="n">
+        <v>390</v>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="1" t="n">
+        <v>271</v>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>Манга "Твое имя", 1 том</t>
+        </is>
+      </c>
+      <c r="C273" t="n">
+        <v>390</v>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Манга "Атака на Титанов", 1 книга</t>
+        </is>
+      </c>
+      <c r="C274" t="n">
+        <v>550</v>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="1" t="n">
+        <v>273</v>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>Манга "Форма голоса", 1 том</t>
+        </is>
+      </c>
+      <c r="C275" t="n">
+        <v>450</v>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="1" t="n">
+        <v>274</v>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>Манга "Волчица и пряности", 1 том</t>
+        </is>
+      </c>
+      <c r="C276" t="n">
+        <v>390</v>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="1" t="n">
+        <v>275</v>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>Манга "Тетрадь смерти: Black Edition", 1 книга</t>
+        </is>
+      </c>
+      <c r="C277" t="n">
+        <v>750</v>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="1" t="n">
+        <v>276</v>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Манга "Госпожа Кагуя: В любви как на войне. Любовная битва двух гениев", 1 книга</t>
+        </is>
+      </c>
+      <c r="C278" t="n">
+        <v>730</v>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="1" t="n">
+        <v>277</v>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>Манга "Созданный в Бездне", 1 том</t>
+        </is>
+      </c>
+      <c r="C279" t="n">
+        <v>420</v>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="1" t="n">
+        <v>278</v>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>Манга "Дракорничная госпожи Кобаяси", 1 том</t>
+        </is>
+      </c>
+      <c r="C280" t="n">
+        <v>390</v>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="1" t="n">
+        <v>279</v>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>Манга "GUNNM", 1 том</t>
+        </is>
+      </c>
+      <c r="C281" t="n">
+        <v>410</v>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="1" t="n">
+        <v>280</v>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>Манга "Дракон в поисках дома", 1 том</t>
+        </is>
+      </c>
+      <c r="C282" t="n">
+        <v>390</v>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="1" t="n">
+        <v>281</v>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>Манга "Невеста чародея", 1 том</t>
+        </is>
+      </c>
+      <c r="C283" t="n">
+        <v>420</v>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="1" t="n">
+        <v>282</v>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>Манга "Излом", 1 том</t>
+        </is>
+      </c>
+      <c r="C284" t="n">
+        <v>450</v>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="1" t="n">
+        <v>283</v>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>Манга "Грань будущего", 1 том</t>
+        </is>
+      </c>
+      <c r="C285" t="n">
+        <v>430</v>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="1" t="n">
+        <v>284</v>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>Манга "Город, в котором меня нет", 1 том</t>
+        </is>
+      </c>
+      <c r="C286" t="n">
+        <v>390</v>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="1" t="n">
+        <v>285</v>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>Манга "Ателье колдовских колпаков", 1 том</t>
+        </is>
+      </c>
+      <c r="C287" t="n">
+        <v>390</v>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="1" t="n">
+        <v>286</v>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>Манга "Хвост феи", 1 том</t>
+        </is>
+      </c>
+      <c r="C288" t="n">
+        <v>390</v>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="1" t="n">
+        <v>287</v>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>Манга "One", 1 том</t>
+        </is>
+      </c>
+      <c r="C289" t="n">
+        <v>310</v>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="1" t="n">
+        <v>288</v>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>Манга "Сейлор Мун", 1 том</t>
+        </is>
+      </c>
+      <c r="C290" t="n">
+        <v>410</v>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="1" t="n">
+        <v>289</v>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>Манга "Милый дом Чи", 1 книга</t>
+        </is>
+      </c>
+      <c r="C291" t="n">
+        <v>390</v>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="1" t="n">
+        <v>290</v>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>Манга "Бакуман", 1 книга</t>
+        </is>
+      </c>
+      <c r="C292" t="n">
+        <v>560</v>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="1" t="n">
+        <v>291</v>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>Манга "У меня мало друзей", 1 том</t>
+        </is>
+      </c>
+      <c r="C293" t="n">
+        <v>390</v>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="1" t="n">
+        <v>292</v>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>Манга "Токийский гуль", 1 книга</t>
+        </is>
+      </c>
+      <c r="C294" t="n">
+        <v>590</v>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="1" t="n">
+        <v>293</v>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>Манга "Блаблабла", 1 том</t>
+        </is>
+      </c>
+      <c r="C295" t="n">
+        <v>420</v>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="1" t="n">
+        <v>294</v>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>Манга "Загадка Дьявола", 1 том</t>
+        </is>
+      </c>
+      <c r="C296" t="n">
+        <v>340</v>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>Манга "Город кислоты", 1 том</t>
+        </is>
+      </c>
+      <c r="C297" t="n">
+        <v>380</v>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="1" t="n">
+        <v>296</v>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>Манга "Летние войны", 1 том</t>
+        </is>
+      </c>
+      <c r="C298" t="n">
+        <v>450</v>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="1" t="n">
+        <v>297</v>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>Манга "Ну не может моя сестренка быть такой милой", 1 том</t>
+        </is>
+      </c>
+      <c r="C299" t="n">
+        <v>380</v>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="1" t="n">
+        <v>298</v>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>Манга "Мобильная маргаритка", 1 том</t>
+        </is>
+      </c>
+      <c r="C300" t="n">
+        <v>390</v>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="1" t="n">
+        <v>299</v>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>Манга "Orange", 1 том</t>
+        </is>
+      </c>
+      <c r="C301" t="n">
+        <v>390</v>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="D267" t="inlineStr">
-        <is>
-          <t>Discomir</t>
-        </is>
-      </c>
-      <c r="E267" t="inlineStr">
-        <is>
-          <t>Pins</t>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Манга "Эльф не может похудеть", 1 том</t>
+        </is>
+      </c>
+      <c r="C302" t="n">
+        <v>320</v>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>Manga</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="n">
+        <v>301</v>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Манга "Шерлок. Скандал в Белгравии", 1 том</t>
+        </is>
+      </c>
+      <c r="C303" t="n">
+        <v>450</v>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>Nyaki</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>Manga</t>
         </is>
       </c>
     </row>

</xml_diff>